<commit_message>
function primer length, structure laboratory
</commit_message>
<xml_diff>
--- a/Strain_characterization.xlsx
+++ b/Strain_characterization.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rwthaachende-my.sharepoint.com/personal/iris_broderius_rwth-aachen_de/Documents/Master/HiWi_Programmieren/GitLab/backup/aktuell_pushen_neu/biolabsim/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_CBEAC7A8C0462EA828E4D0D0FC2D62B13037D478" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A748C98E-E140-45F8-8F8B-7FF4CF4D48A8}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="different temp" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -37,8 +43,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,15 +103,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -147,7 +161,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,9 +193,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,6 +245,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -388,14 +438,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -418,7 +471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -426,10 +479,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.1190037264585485</v>
+        <v>0.11900372645854849</v>
       </c>
       <c r="D2">
-        <v>0.08706597667908471</v>
+        <v>8.7065976679084708E-2</v>
       </c>
       <c r="E2">
         <v>0.1001184595134543</v>
@@ -438,13 +491,13 @@
         <v>0.1060003823740093</v>
       </c>
       <c r="G2">
-        <v>0.08023766677395397</v>
+        <v>8.023766677395397E-2</v>
       </c>
       <c r="H2">
         <v>0.1060003823740093</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -452,25 +505,25 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.2520467972112088</v>
+        <v>0.25204679721120882</v>
       </c>
       <c r="D3">
-        <v>0.208945417304096</v>
+        <v>0.20894541730409599</v>
       </c>
       <c r="E3">
-        <v>0.2722326467960313</v>
+        <v>0.27223264679603132</v>
       </c>
       <c r="F3">
         <v>0.1748414316230166</v>
       </c>
       <c r="G3">
-        <v>0.1925584873341027</v>
+        <v>0.19255848733410269</v>
       </c>
       <c r="H3">
         <v>0.1748414316230166</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -478,25 +531,25 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.5329272241481693</v>
+        <v>0.53292722414816929</v>
       </c>
       <c r="D4">
-        <v>0.5001118476061661</v>
+        <v>0.50011184760616612</v>
       </c>
       <c r="E4">
-        <v>0.7372808194991082</v>
+        <v>0.73728081949910818</v>
       </c>
       <c r="F4">
         <v>0.2882262151785312</v>
       </c>
       <c r="G4">
-        <v>0.4608896529793325</v>
+        <v>0.46088965297933249</v>
       </c>
       <c r="H4">
         <v>0.2882262151785312</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -504,7 +557,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>1.122817786753349</v>
+        <v>1.1228177867533491</v>
       </c>
       <c r="D5">
         <v>1.189504777287681</v>
@@ -513,16 +566,16 @@
         <v>1.975497999753308</v>
       </c>
       <c r="F5">
-        <v>0.4746951311386213</v>
+        <v>0.47469513113862127</v>
       </c>
       <c r="G5">
         <v>1.096215669845727</v>
       </c>
       <c r="H5">
-        <v>0.4746951311386213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>0.47469513113862127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -536,19 +589,19 @@
         <v>2.787769615459923</v>
       </c>
       <c r="E6">
-        <v>5.147296131505654</v>
+        <v>5.1472961315056542</v>
       </c>
       <c r="F6">
-        <v>0.7805957978551002</v>
+        <v>0.78059579785510025</v>
       </c>
       <c r="G6">
-        <v>2.569133638416547</v>
+        <v>2.5691336384165471</v>
       </c>
       <c r="H6">
-        <v>0.7805957978551002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>0.78059579785510025</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -556,25 +609,25 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>4.83624089375625</v>
+        <v>4.8362408937562504</v>
       </c>
       <c r="D7">
-        <v>6.318945445802083</v>
+        <v>6.3189454458020826</v>
       </c>
       <c r="E7">
-        <v>12.52698270878085</v>
+        <v>12.526982708780849</v>
       </c>
       <c r="F7">
-        <v>1.280386136742588</v>
+        <v>1.2803861367425879</v>
       </c>
       <c r="G7">
-        <v>5.82337048732446</v>
+        <v>5.8233704873244596</v>
       </c>
       <c r="H7">
-        <v>1.280386136742588</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>1.2803861367425879</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -582,25 +635,25 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>9.663536345425412</v>
+        <v>9.6635363454254115</v>
       </c>
       <c r="D8">
-        <v>13.35395029569417</v>
+        <v>13.353950295694171</v>
       </c>
       <c r="E8">
-        <v>26.43063205536304</v>
+        <v>26.430632055363041</v>
       </c>
       <c r="F8">
-        <v>2.091557784354451</v>
+        <v>2.0915577843544511</v>
       </c>
       <c r="G8">
-        <v>12.30664209845417</v>
+        <v>12.306642098454169</v>
       </c>
       <c r="H8">
-        <v>2.091557784354451</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>2.0915577843544511</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -608,25 +661,25 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>18.25247827848231</v>
+        <v>18.252478278482311</v>
       </c>
       <c r="D9">
-        <v>24.86922138620484</v>
+        <v>24.869221386204838</v>
       </c>
       <c r="E9">
-        <v>44.58869976070628</v>
+        <v>44.588699760706277</v>
       </c>
       <c r="F9">
-        <v>3.394031244817859</v>
+        <v>3.3940312448178589</v>
       </c>
       <c r="G9">
-        <v>22.91880680175437</v>
+        <v>22.918806801754371</v>
       </c>
       <c r="H9">
-        <v>3.394031244817859</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>3.3940312448178589</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -634,25 +687,25 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>31.41622156921306</v>
+        <v>31.416221569213061</v>
       </c>
       <c r="D10">
         <v>38.77565348470695</v>
       </c>
       <c r="E10">
-        <v>59.61629824248197</v>
+        <v>59.616298242481967</v>
       </c>
       <c r="F10">
-        <v>5.449697895706599</v>
+        <v>5.4496978957065991</v>
       </c>
       <c r="G10">
-        <v>35.7346012980019</v>
+        <v>35.734601298001898</v>
       </c>
       <c r="H10">
-        <v>5.449697895706599</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>5.4496978957065991</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -660,25 +713,25 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>47.60036496365675</v>
+        <v>47.600364963656752</v>
       </c>
       <c r="D11">
-        <v>50.52635106434222</v>
+        <v>50.526351064342222</v>
       </c>
       <c r="E11">
-        <v>68.02868752519544</v>
+        <v>68.028687525195437</v>
       </c>
       <c r="F11">
-        <v>8.607617409838243</v>
+        <v>8.6076174098382428</v>
       </c>
       <c r="G11">
-        <v>46.56372873352721</v>
+        <v>46.563728733527213</v>
       </c>
       <c r="H11">
-        <v>8.607617409838243</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>8.6076174098382428</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -686,25 +739,25 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>62.86872026200478</v>
+        <v>62.868720262004778</v>
       </c>
       <c r="D12">
-        <v>57.81289184804034</v>
+        <v>57.812891848040337</v>
       </c>
       <c r="E12">
-        <v>71.74316187110074</v>
+        <v>71.743161871100739</v>
       </c>
       <c r="F12">
         <v>13.26293835898394</v>
       </c>
       <c r="G12">
-        <v>53.27880910863362</v>
+        <v>53.278809108633617</v>
       </c>
       <c r="H12">
         <v>13.26293835898394</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -712,25 +765,25 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>74.06934813264667</v>
+        <v>74.069348132646667</v>
       </c>
       <c r="D13">
-        <v>61.50167017404566</v>
+        <v>61.501670174045657</v>
       </c>
       <c r="E13">
-        <v>73.20984829684238</v>
+        <v>73.209848296842381</v>
       </c>
       <c r="F13">
-        <v>19.72486357996264</v>
+        <v>19.724863579962641</v>
       </c>
       <c r="G13">
-        <v>56.67828818661999</v>
+        <v>56.678288186619987</v>
       </c>
       <c r="H13">
-        <v>19.72486357996264</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>19.724863579962641</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -738,25 +791,25 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>80.86088580392615</v>
+        <v>80.860885803926152</v>
       </c>
       <c r="D14">
-        <v>63.17822383674066</v>
+        <v>63.178223836740663</v>
       </c>
       <c r="E14">
-        <v>73.76314576629088</v>
+        <v>73.763145766290876</v>
       </c>
       <c r="F14">
         <v>27.98342201698312</v>
       </c>
       <c r="G14">
-        <v>58.22335503416492</v>
+        <v>58.223355034164918</v>
       </c>
       <c r="H14">
         <v>27.98342201698312</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -764,25 +817,25 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>84.51414832740184</v>
+        <v>84.514148327401841</v>
       </c>
       <c r="D15">
-        <v>63.90273010045818</v>
+        <v>63.902730100458179</v>
       </c>
       <c r="E15">
-        <v>73.96826060405714</v>
+        <v>73.968260604057136</v>
       </c>
       <c r="F15">
-        <v>37.49183928052153</v>
+        <v>37.491839280521532</v>
       </c>
       <c r="G15">
-        <v>58.89104055704236</v>
+        <v>58.891040557042359</v>
       </c>
       <c r="H15">
-        <v>37.49183928052153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>37.491839280521532</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -790,22 +843,22 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>86.35341099217852</v>
+        <v>86.353410992178524</v>
       </c>
       <c r="D16">
-        <v>64.20897059856323</v>
+        <v>64.208970598563226</v>
       </c>
       <c r="F16">
-        <v>47.20826955552197</v>
+        <v>47.208269555521973</v>
       </c>
       <c r="G16">
         <v>59.17326357890326</v>
       </c>
       <c r="H16">
-        <v>47.20826955552197</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>47.208269555521973</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -813,22 +866,22 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>87.24855820916748</v>
+        <v>87.248558209167484</v>
       </c>
       <c r="D17">
-        <v>64.33720293888912</v>
+        <v>64.337202938889121</v>
       </c>
       <c r="F17">
-        <v>55.9991572151178</v>
+        <v>55.999157215117798</v>
       </c>
       <c r="G17">
-        <v>59.2914390612807</v>
+        <v>59.291439061280698</v>
       </c>
       <c r="H17">
-        <v>55.9991572151178</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>55.999157215117798</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -836,16 +889,16 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>87.67703043127715</v>
+        <v>87.677030431277146</v>
       </c>
       <c r="F18">
-        <v>63.11873394912603</v>
+        <v>63.118733949126032</v>
       </c>
       <c r="H18">
-        <v>63.11873394912603</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>63.118733949126032</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -853,16 +906,16 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>87.88049029774034</v>
+        <v>87.880490297740337</v>
       </c>
       <c r="F19">
-        <v>68.38515748464319</v>
+        <v>68.385157484643187</v>
       </c>
       <c r="H19">
-        <v>68.38515748464319</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>68.385157484643187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -870,13 +923,13 @@
         <v>18</v>
       </c>
       <c r="F20">
-        <v>72.02534802389428</v>
+        <v>72.025348023894281</v>
       </c>
       <c r="H20">
-        <v>72.02534802389428</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>72.025348023894281</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -884,13 +937,13 @@
         <v>19</v>
       </c>
       <c r="F21">
-        <v>74.42508048085443</v>
+        <v>74.425080480854433</v>
       </c>
       <c r="H21">
-        <v>74.42508048085443</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>74.425080480854433</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -898,13 +951,13 @@
         <v>20</v>
       </c>
       <c r="F22">
-        <v>75.958046378402</v>
+        <v>75.958046378402003</v>
       </c>
       <c r="H22">
-        <v>75.958046378402</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>75.958046378402003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -912,13 +965,13 @@
         <v>21</v>
       </c>
       <c r="F23">
-        <v>76.91771389746569</v>
+        <v>76.917713897465688</v>
       </c>
       <c r="H23">
-        <v>76.91771389746569</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>76.917713897465688</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -926,13 +979,13 @@
         <v>22</v>
       </c>
       <c r="F24">
-        <v>77.51090009495853</v>
+        <v>77.510900094958529</v>
       </c>
       <c r="H24">
-        <v>77.51090009495853</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>77.510900094958529</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -940,13 +993,13 @@
         <v>23</v>
       </c>
       <c r="F25">
-        <v>77.87468293401376</v>
+        <v>77.874682934013762</v>
       </c>
       <c r="H25">
-        <v>77.87468293401376</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>77.874682934013762</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -960,7 +1013,7 @@
         <v>78.09670358827168</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -968,13 +1021,13 @@
         <v>25</v>
       </c>
       <c r="F27">
-        <v>78.23180556011793</v>
+        <v>78.231805560117934</v>
       </c>
       <c r="H27">
-        <v>78.23180556011793</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>78.231805560117934</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -982,10 +1035,10 @@
         <v>26</v>
       </c>
       <c r="F28">
-        <v>78.31386884770004</v>
+        <v>78.313868847700036</v>
       </c>
       <c r="H28">
-        <v>78.31386884770004</v>
+        <v>78.313868847700036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Temp-Vector randomization test, vol2
</commit_message>
<xml_diff>
--- a/Strain_characterization.xlsx
+++ b/Strain_characterization.xlsx
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H110"/>
+  <dimension ref="A1:H105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -426,22 +426,22 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.09049460440025167</v>
+        <v>0.09644718297262804</v>
       </c>
       <c r="D2">
-        <v>0.1124517843076147</v>
+        <v>0.09668237232779985</v>
       </c>
       <c r="E2">
-        <v>0.0975719587492303</v>
+        <v>0.1002355349273059</v>
       </c>
       <c r="F2">
-        <v>0.09737822604539416</v>
+        <v>0.1021898834130745</v>
       </c>
       <c r="G2">
-        <v>0.1038775756951044</v>
+        <v>0.09635915738830481</v>
       </c>
       <c r="H2">
-        <v>0.09737822604539416</v>
+        <v>0.1021898834130745</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -452,22 +452,22 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.1025626771729137</v>
+        <v>0.2621656159582414</v>
       </c>
       <c r="D3">
-        <v>0.144441261349066</v>
+        <v>0.2319624997735628</v>
       </c>
       <c r="E3">
-        <v>0.1420360808043341</v>
+        <v>0.1873218221187095</v>
       </c>
       <c r="F3">
-        <v>0.2649022300718269</v>
+        <v>0.1158106207244724</v>
       </c>
       <c r="G3">
-        <v>0.2200751426198456</v>
+        <v>0.1237548068717991</v>
       </c>
       <c r="H3">
-        <v>0.2649022300718269</v>
+        <v>0.1158106207244724</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -478,22 +478,22 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.1162378603891302</v>
+        <v>0.7093993427177036</v>
       </c>
       <c r="D4">
-        <v>0.1855145394394496</v>
+        <v>0.5548557725168748</v>
       </c>
       <c r="E4">
-        <v>0.2067160558353938</v>
+        <v>0.3496634247721204</v>
       </c>
       <c r="F4">
-        <v>0.7183117973391346</v>
+        <v>0.131243253145877</v>
       </c>
       <c r="G4">
-        <v>0.4656174683565285</v>
+        <v>0.1589194572789361</v>
       </c>
       <c r="H4">
-        <v>0.7183117973391346</v>
+        <v>0.131243253145877</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -504,22 +504,22 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0.1317335339755265</v>
+        <v>1.896402172042379</v>
       </c>
       <c r="D5">
-        <v>0.2382404701279599</v>
+        <v>1.3177587422085</v>
       </c>
       <c r="E5">
-        <v>0.3007509709463447</v>
+        <v>0.6512871819876905</v>
       </c>
       <c r="F5">
-        <v>1.93100511314563</v>
+        <v>0.1487277866450297</v>
       </c>
       <c r="G5">
-        <v>0.9822939996159402</v>
+        <v>0.204043448484679</v>
       </c>
       <c r="H5">
-        <v>1.93100511314563</v>
+        <v>0.1487277866450297</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -530,22 +530,22 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>0.1492912269950622</v>
+        <v>4.912151142362099</v>
       </c>
       <c r="D6">
-        <v>0.3059074872113278</v>
+        <v>3.077789839228751</v>
       </c>
       <c r="E6">
-        <v>0.4373533759466178</v>
+        <v>1.208244047846321</v>
       </c>
       <c r="F6">
-        <v>5.074138208506866</v>
+        <v>0.1685357287420055</v>
       </c>
       <c r="G6">
-        <v>2.059886875685248</v>
+        <v>0.2619263421834881</v>
       </c>
       <c r="H6">
-        <v>5.074138208506866</v>
+        <v>0.1685357287420055</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -556,22 +556,22 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.1691842793950329</v>
+        <v>11.79336209047015</v>
       </c>
       <c r="D7">
-        <v>0.3927207212322942</v>
+        <v>6.924013275159183</v>
       </c>
       <c r="E7">
-        <v>0.6355604210206703</v>
+        <v>2.225059852694149</v>
       </c>
       <c r="F7">
-        <v>12.5981134334901</v>
+        <v>0.190974140826587</v>
       </c>
       <c r="G7">
-        <v>4.266296322044787</v>
+        <v>0.336141000344697</v>
       </c>
       <c r="H7">
-        <v>12.5981134334901</v>
+        <v>0.190974140826587</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -582,22 +582,22 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>0.1917219653659137</v>
+        <v>24.26573549000705</v>
       </c>
       <c r="D8">
-        <v>0.5040502223036918</v>
+        <v>14.41727541471812</v>
       </c>
       <c r="E8">
-        <v>0.9226664077284579</v>
+        <v>4.0434818841954</v>
       </c>
       <c r="F8">
-        <v>27.63113525952549</v>
+        <v>0.2163901883017268</v>
       </c>
       <c r="G8">
-        <v>8.618238513537339</v>
+        <v>0.4312383778942696</v>
       </c>
       <c r="H8">
-        <v>27.63113525952549</v>
+        <v>0.2163901883017268</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -608,22 +608,22 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>0.2172541322811146</v>
+        <v>39.65233979744736</v>
       </c>
       <c r="D9">
-        <v>0.64674165705992</v>
+        <v>26.21780736385123</v>
       </c>
       <c r="E9">
-        <v>1.337522450435575</v>
+        <v>7.178476880213952</v>
       </c>
       <c r="F9">
-        <v>49.15065528389117</v>
+        <v>0.2451762429628532</v>
       </c>
       <c r="G9">
-        <v>16.60224179258215</v>
+        <v>0.5530008565624496</v>
       </c>
       <c r="H9">
-        <v>49.15065528389117</v>
+        <v>0.2451762429628532</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -634,22 +634,22 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>0.24617641426246</v>
+        <v>51.67470176632608</v>
       </c>
       <c r="D10">
-        <v>0.8295021030917203</v>
+        <v>39.74903322011231</v>
       </c>
       <c r="E10">
-        <v>1.934846822497746</v>
+        <v>12.25659393354364</v>
       </c>
       <c r="F10">
-        <v>68.81499884390669</v>
+        <v>0.2777755959683427</v>
       </c>
       <c r="G10">
-        <v>29.47532996878604</v>
+        <v>0.7087518868798387</v>
       </c>
       <c r="H10">
-        <v>68.81499884390669</v>
+        <v>0.2777755959683427</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -660,22 +660,22 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>0.2789360845848116</v>
+        <v>58.14284709420083</v>
       </c>
       <c r="D11">
-        <v>1.063373998019494</v>
+        <v>50.61321051349171</v>
       </c>
       <c r="E11">
-        <v>2.790512359754106</v>
+        <v>19.70596665044129</v>
       </c>
       <c r="F11">
-        <v>80.65475033153311</v>
+        <v>0.3146888433354237</v>
       </c>
       <c r="G11">
-        <v>46.45753273526417</v>
+        <v>0.9077283151067743</v>
       </c>
       <c r="H11">
-        <v>80.65475033153311</v>
+        <v>0.3146888433354237</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -686,22 +686,22 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>0.3160386162524541</v>
+        <v>60.94169172717419</v>
       </c>
       <c r="D12">
-        <v>1.362309020615426</v>
+        <v>57.10453056994955</v>
       </c>
       <c r="E12">
-        <v>4.007321945675375</v>
+        <v>29.1849066332236</v>
       </c>
       <c r="F12">
-        <v>86.08940136172535</v>
+        <v>0.3564810088277913</v>
       </c>
       <c r="G12">
-        <v>63.7817514634709</v>
+        <v>1.161518003114779</v>
       </c>
       <c r="H12">
-        <v>86.08940136172535</v>
+        <v>0.3564810088277913</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -712,22 +712,22 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>0.3580550249475784</v>
+        <v>62.03740934598493</v>
       </c>
       <c r="D13">
-        <v>1.743849237115394</v>
+        <v>60.32217704342734</v>
       </c>
       <c r="E13">
-        <v>5.719830596253988</v>
+        <v>39.28233823176495</v>
       </c>
       <c r="F13">
-        <v>88.27175932877365</v>
+        <v>0.4037894710127932</v>
       </c>
       <c r="G13">
-        <v>77.38627476088519</v>
+        <v>1.484557605448819</v>
       </c>
       <c r="H13">
-        <v>88.27175932877365</v>
+        <v>0.4037894710127932</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -738,22 +738,22 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>0.405630072889317</v>
+        <v>62.44938810122754</v>
       </c>
       <c r="D14">
-        <v>2.229912982591492</v>
+        <v>61.76973404560346</v>
       </c>
       <c r="E14">
-        <v>8.095090851966459</v>
+        <v>48.19245061311514</v>
       </c>
       <c r="F14">
-        <v>89.10050054613076</v>
+        <v>0.4573327616665871</v>
       </c>
       <c r="G14">
-        <v>86.03791908088324</v>
+        <v>1.894671360377789</v>
       </c>
       <c r="H14">
-        <v>89.10050054613076</v>
+        <v>0.4573327616665871</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -763,23 +763,20 @@
       <c r="B15">
         <v>13</v>
       </c>
-      <c r="C15">
-        <v>0.4594914155751206</v>
-      </c>
       <c r="D15">
-        <v>2.847664350056004</v>
+        <v>62.39243971303532</v>
       </c>
       <c r="E15">
-        <v>11.32382326374979</v>
+        <v>54.83953467745111</v>
       </c>
       <c r="F15">
-        <v>89.40849182576794</v>
+        <v>0.5179203009588064</v>
       </c>
       <c r="G15">
-        <v>90.82489789059325</v>
+        <v>2.413608466277282</v>
       </c>
       <c r="H15">
-        <v>89.40849182576794</v>
+        <v>0.5179203009588064</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -789,1249 +786,1395 @@
       <c r="B16">
         <v>14</v>
       </c>
-      <c r="C16">
-        <v>0.5204597754064945</v>
-      </c>
       <c r="D16">
-        <v>3.630413297686251</v>
+        <v>62.65513722237957</v>
       </c>
       <c r="E16">
-        <v>15.59444606298139</v>
+        <v>59.20317251882064</v>
+      </c>
+      <c r="F16">
+        <v>0.5864631301384318</v>
       </c>
       <c r="G16">
-        <v>93.2713790527532</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>3.067500604151937</v>
+      </c>
+      <c r="H16">
+        <v>0.5864631301384318</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
         <v>15</v>
       </c>
-      <c r="C17">
-        <v>0.5894602261756547</v>
-      </c>
-      <c r="D17">
-        <v>4.618442725377928</v>
-      </c>
       <c r="E17">
-        <v>21.04360048329548</v>
+        <v>61.83236483367854</v>
+      </c>
+      <c r="F17">
+        <v>0.6639856937364554</v>
       </c>
       <c r="G17">
-        <v>94.47103721254315</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>3.887109572054599</v>
+      </c>
+      <c r="H17">
+        <v>0.6639856937364554</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
         <v>16</v>
       </c>
-      <c r="C18">
-        <v>0.6675346694643683</v>
-      </c>
-      <c r="D18">
-        <v>5.859584000883828</v>
-      </c>
       <c r="E18">
-        <v>27.68610704080845</v>
+        <v>63.33542236668426</v>
+      </c>
+      <c r="F18">
+        <v>0.7516387093048389</v>
       </c>
       <c r="G18">
-        <v>95.04736701239347</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>4.907667911631417</v>
+      </c>
+      <c r="H18">
+        <v>0.7516387093048389</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
         <v>17</v>
       </c>
-      <c r="C19">
-        <v>0.7558555771019809</v>
-      </c>
-      <c r="D19">
-        <v>7.409260940146368</v>
-      </c>
       <c r="E19">
-        <v>35.34691092833006</v>
+        <v>64.16898157508274</v>
+      </c>
+      <c r="F19">
+        <v>0.8507131418254698</v>
       </c>
       <c r="G19">
-        <v>95.32151508689441</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>6.16804029617857</v>
+      </c>
+      <c r="H19">
+        <v>0.8507131418254698</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
         <v>18</v>
       </c>
-      <c r="C20">
-        <v>0.855741061582888</v>
-      </c>
-      <c r="D20">
-        <v>9.329600656838899</v>
-      </c>
       <c r="E20">
-        <v>43.63744953907162</v>
+        <v>64.62347926263483</v>
+      </c>
+      <c r="F20">
+        <v>0.9626552701961073</v>
       </c>
       <c r="G20">
-        <v>95.45130736687241</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>7.708871839815442</v>
+      </c>
+      <c r="H20">
+        <v>0.9626552701961073</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
         <v>19</v>
       </c>
-      <c r="C21">
-        <v>0.9686713170518365</v>
-      </c>
-      <c r="D21">
-        <v>11.68709304617734</v>
-      </c>
       <c r="E21">
-        <v>52.01393701885989</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>64.8690040369187</v>
+      </c>
+      <c r="F21">
+        <v>1.089082792289447</v>
+      </c>
+      <c r="G21">
+        <v>9.56938427341013</v>
+      </c>
+      <c r="H21">
+        <v>1.089082792289447</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22">
         <v>20</v>
       </c>
-      <c r="C22">
-        <v>1.096306445029341</v>
-      </c>
-      <c r="D22">
-        <v>14.5482249167826</v>
-      </c>
       <c r="E22">
-        <v>59.91004681331561</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>65.00097439962995</v>
+      </c>
+      <c r="F22">
+        <v>1.231801860223536</v>
+      </c>
+      <c r="G22">
+        <v>11.78259850404748</v>
+      </c>
+      <c r="H22">
+        <v>1.231801860223536</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23">
         <v>21</v>
       </c>
-      <c r="C23">
-        <v>1.240505638917261</v>
-      </c>
-      <c r="D23">
-        <v>17.97261536563084</v>
-      </c>
-      <c r="E23">
-        <v>66.88126840029096</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="F23">
+        <v>1.392824865491286</v>
+      </c>
+      <c r="G23">
+        <v>14.36907760276277</v>
+      </c>
+      <c r="H23">
+        <v>1.392824865491286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24">
         <v>22</v>
       </c>
-      <c r="C24">
-        <v>1.403347646443279</v>
-      </c>
-      <c r="D24">
-        <v>22.00356014601566</v>
-      </c>
-      <c r="E24">
-        <v>72.6887430535361</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="F24">
+        <v>1.574388700904317</v>
+      </c>
+      <c r="G24">
+        <v>17.32983600666847</v>
+      </c>
+      <c r="H24">
+        <v>1.574388700904317</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25">
         <v>23</v>
       </c>
-      <c r="C25">
-        <v>1.587152355989677</v>
-      </c>
-      <c r="D25">
-        <v>26.65665419418486</v>
-      </c>
-      <c r="E25">
-        <v>77.29722240423347</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="F25">
+        <v>1.778973109063065</v>
+      </c>
+      <c r="G25">
+        <v>20.63977203596981</v>
+      </c>
+      <c r="H25">
+        <v>1.778973109063065</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26">
         <v>24</v>
       </c>
-      <c r="C26">
-        <v>1.794503257098943</v>
-      </c>
-      <c r="D26">
-        <v>31.90826726428799</v>
-      </c>
-      <c r="E26">
-        <v>80.81521189972469</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="F26">
+        <v>2.009318581345303</v>
+      </c>
+      <c r="G26">
+        <v>24.24358859592775</v>
+      </c>
+      <c r="H26">
+        <v>2.009318581345303</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27">
         <v>25</v>
       </c>
-      <c r="C27">
-        <v>2.028270402788782</v>
-      </c>
-      <c r="D27">
-        <v>37.68679043065033</v>
-      </c>
-      <c r="E27">
-        <v>83.4221019465372</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="F27">
+        <v>2.268443093547913</v>
+      </c>
+      <c r="G27">
+        <v>28.05624785335158</v>
+      </c>
+      <c r="H27">
+        <v>2.268443093547913</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28">
         <v>26</v>
       </c>
-      <c r="C28">
-        <v>2.291633346769117</v>
-      </c>
-      <c r="D28">
-        <v>43.87013141626466</v>
-      </c>
-      <c r="E28">
-        <v>85.31160966246605</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="F28">
+        <v>2.559656751457029</v>
+      </c>
+      <c r="G28">
+        <v>31.9691891527128</v>
+      </c>
+      <c r="H28">
+        <v>2.559656751457029</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29">
         <v>27</v>
       </c>
-      <c r="C29">
-        <v>2.588103337342837</v>
-      </c>
-      <c r="D29">
-        <v>50.29220614412244</v>
-      </c>
-      <c r="E29">
-        <v>86.65931115525846</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="F29">
+        <v>2.886573170470111</v>
+      </c>
+      <c r="G29">
+        <v>35.8618549237307</v>
+      </c>
+      <c r="H29">
+        <v>2.886573170470111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30">
         <v>28</v>
       </c>
-      <c r="C30">
-        <v>2.921543817257898</v>
-      </c>
-      <c r="D30">
-        <v>56.75887835526527</v>
-      </c>
-      <c r="E30">
-        <v>87.60958357490777</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="F30">
+        <v>3.253116129322523</v>
+      </c>
+      <c r="G30">
+        <v>39.61614983032884</v>
+      </c>
+      <c r="H30">
+        <v>3.253116129322523</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31">
         <v>29</v>
       </c>
-      <c r="C31">
-        <v>3.296188001815853</v>
-      </c>
-      <c r="D31">
-        <v>63.070598531435</v>
-      </c>
-      <c r="E31">
-        <v>88.27421009657215</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="F31">
+        <v>3.66351972446038</v>
+      </c>
+      <c r="G31">
+        <v>43.13028609302875</v>
+      </c>
+      <c r="H31">
+        <v>3.66351972446038</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32">
         <v>30</v>
       </c>
-      <c r="C32">
-        <v>3.716651985129903</v>
-      </c>
-      <c r="D32">
-        <v>69.04639148861209</v>
-      </c>
-      <c r="E32">
-        <v>88.73641961913516</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32">
+        <v>4.122319920061033</v>
+      </c>
+      <c r="G32">
+        <v>46.32871902090505</v>
+      </c>
+      <c r="H32">
+        <v>4.122319920061033</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33">
         <v>31</v>
       </c>
-      <c r="C33">
-        <v>4.187941459265685</v>
-      </c>
-      <c r="D33">
-        <v>74.54329070042353</v>
-      </c>
-      <c r="E33">
-        <v>89.05659066097901</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33">
+        <v>4.634335058644196</v>
+      </c>
+      <c r="G33">
+        <v>49.16640259029277</v>
+      </c>
+      <c r="H33">
+        <v>4.634335058644196</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34">
         <v>32</v>
       </c>
-      <c r="C34">
-        <v>4.71544973141097</v>
-      </c>
-      <c r="D34">
-        <v>79.46714292696609</v>
-      </c>
-      <c r="E34">
-        <v>89.27776482362857</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34">
+        <v>5.204632598630116</v>
+      </c>
+      <c r="G34">
+        <v>51.62753920877371</v>
+      </c>
+      <c r="H34">
+        <v>5.204632598630116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35">
         <v>33</v>
       </c>
-      <c r="C35">
-        <v>5.304944306537696</v>
-      </c>
-      <c r="D35">
-        <v>83.77385224432985</v>
-      </c>
-      <c r="E35">
-        <v>89.43026269040678</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35">
+        <v>5.83847912085281</v>
+      </c>
+      <c r="G35">
+        <v>53.72043414231373</v>
+      </c>
+      <c r="H35">
+        <v>5.83847912085281</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36">
         <v>34</v>
       </c>
-      <c r="C36">
-        <v>5.962538894381772</v>
-      </c>
-      <c r="D36">
-        <v>87.46297254617627</v>
-      </c>
-      <c r="E36">
-        <v>89.53527145523211</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36">
+        <v>6.541270553182885</v>
+      </c>
+      <c r="G36">
+        <v>55.47055955880168</v>
+      </c>
+      <c r="H36">
+        <v>6.541270553182885</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37">
         <v>35</v>
       </c>
-      <c r="C37">
-        <v>6.694647340920337</v>
-      </c>
-      <c r="D37">
-        <v>90.56699543626996</v>
-      </c>
-      <c r="E37">
-        <v>89.60751456139523</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37">
+        <v>7.318439673161032</v>
+      </c>
+      <c r="G37">
+        <v>56.91362671696504</v>
+      </c>
+      <c r="H37">
+        <v>7.318439673161032</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38">
         <v>36</v>
       </c>
-      <c r="C38">
-        <v>7.507915733408187</v>
-      </c>
-      <c r="D38">
-        <v>93.13961607226322</v>
-      </c>
-      <c r="E38">
-        <v>89.65718503381959</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38">
+        <v>8.175338347787225</v>
+      </c>
+      <c r="G38">
+        <v>58.08978117841212</v>
+      </c>
+      <c r="H38">
+        <v>8.175338347787225</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39">
         <v>37</v>
       </c>
-      <c r="C39">
-        <v>8.40912886043375</v>
-      </c>
-      <c r="D39">
-        <v>95.2452840556103</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39">
+        <v>9.117092749279239</v>
+      </c>
+      <c r="G39">
+        <v>59.03935854185432</v>
+      </c>
+      <c r="H39">
+        <v>9.117092749279239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40">
         <v>38</v>
       </c>
-      <c r="C40">
-        <v>9.405087418707447</v>
-      </c>
-      <c r="D40">
-        <v>96.95116655195285</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40">
+        <v>10.14843103384565</v>
+      </c>
+      <c r="G40">
+        <v>59.80016398518538</v>
+      </c>
+      <c r="H40">
+        <v>10.14843103384565</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41">
         <v>39</v>
       </c>
-      <c r="C41">
-        <v>10.50245295561916</v>
-      </c>
-      <c r="D41">
-        <v>98.32171918732467</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41">
+        <v>11.27348475476635</v>
+      </c>
+      <c r="G41">
+        <v>60.40599661227983</v>
+      </c>
+      <c r="H41">
+        <v>11.27348475476635</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42">
         <v>40</v>
       </c>
-      <c r="C42">
-        <v>11.70755863658605</v>
-      </c>
-      <c r="D42">
-        <v>99.41551809115444</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42">
+        <v>12.49556762498024</v>
+      </c>
+      <c r="G42">
+        <v>60.88607135695089</v>
+      </c>
+      <c r="H42">
+        <v>12.49556762498024</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43">
         <v>41</v>
       </c>
-      <c r="C43">
-        <v>13.02618563564114</v>
-      </c>
-      <c r="D43">
-        <v>100.2837973247441</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43">
+        <v>13.81693809996247</v>
+      </c>
+      <c r="G43">
+        <v>61.26502145102876</v>
+      </c>
+      <c r="H43">
+        <v>13.81693809996247</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44">
         <v>42</v>
       </c>
-      <c r="C44">
-        <v>14.46330734158492</v>
-      </c>
-      <c r="D44">
-        <v>100.9701365201217</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44">
+        <v>15.23855547078461</v>
+      </c>
+      <c r="G44">
+        <v>61.56323413903845</v>
+      </c>
+      <c r="H44">
+        <v>15.23855547078461</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45">
         <v>43</v>
       </c>
-      <c r="C45">
-        <v>16.02280666298881</v>
-      </c>
-      <c r="D45">
-        <v>101.51084239239</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45">
+        <v>16.75984246925367</v>
+      </c>
+      <c r="G45">
+        <v>61.79734630185648</v>
+      </c>
+      <c r="H45">
+        <v>16.75984246925367</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46">
         <v>44</v>
       </c>
-      <c r="C46">
-        <v>17.70717541807824</v>
-      </c>
-      <c r="D46">
-        <v>101.9356918236079</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46">
+        <v>18.37847039231261</v>
+      </c>
+      <c r="G46">
+        <v>61.98078893428114</v>
+      </c>
+      <c r="H46">
+        <v>18.37847039231261</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47">
         <v>45</v>
       </c>
-      <c r="C47">
-        <v>19.51720889181997</v>
-      </c>
-      <c r="D47">
-        <v>102.2688162373259</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47">
+        <v>20.09018494300416</v>
+      </c>
+      <c r="G47">
+        <v>62.12431563082048</v>
+      </c>
+      <c r="H47">
+        <v>20.09018494300416</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48">
         <v>46</v>
       </c>
-      <c r="C48">
-        <v>21.45171275662649</v>
-      </c>
-      <c r="D48">
-        <v>102.5295936951337</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="F48">
+        <v>21.88869179842145</v>
+      </c>
+      <c r="G48">
+        <v>62.23648163424986</v>
+      </c>
+      <c r="H48">
+        <v>21.88869179842145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49">
         <v>47</v>
       </c>
-      <c r="C49">
-        <v>23.50724314984094</v>
-      </c>
-      <c r="D49">
-        <v>102.7334759483092</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="F49">
+        <v>23.76561982904795</v>
+      </c>
+      <c r="G49">
+        <v>62.32405982879263</v>
+      </c>
+      <c r="H49">
+        <v>23.76561982904795</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50">
         <v>48</v>
       </c>
-      <c r="C50">
-        <v>25.67790312050845</v>
-      </c>
-      <c r="D50">
-        <v>102.8927171505802</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="F50">
+        <v>25.71057654799594</v>
+      </c>
+      <c r="G50">
+        <v>62.39239168402996</v>
+      </c>
+      <c r="H50">
+        <v>25.71057654799594</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51">
         <v>49</v>
       </c>
-      <c r="C51">
-        <v>27.95521919511827</v>
-      </c>
-      <c r="D51">
-        <v>103.0169947813933</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="F51">
+        <v>27.71130469135201</v>
+      </c>
+      <c r="G51">
+        <v>62.44567736016472</v>
+      </c>
+      <c r="H51">
+        <v>27.71130469135201</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52">
         <v>50</v>
       </c>
-      <c r="C52">
-        <v>30.32811984385696</v>
-      </c>
-      <c r="D52">
-        <v>103.1139265815252</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="F52">
+        <v>29.75394113907327</v>
+      </c>
+      <c r="G52">
+        <v>62.48721201627314</v>
+      </c>
+      <c r="H52">
+        <v>29.75394113907327</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53">
         <v>51</v>
       </c>
-      <c r="C53">
-        <v>32.78303277124068</v>
-      </c>
-      <c r="D53">
-        <v>103.1894938122979</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="F53">
+        <v>31.8233704173977</v>
+      </c>
+      <c r="G53">
+        <v>62.51957621709784</v>
+      </c>
+      <c r="H53">
+        <v>31.8233704173977</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54">
         <v>52</v>
       </c>
-      <c r="C54">
-        <v>35.30411021884598</v>
-      </c>
-      <c r="D54">
-        <v>103.2483836106597</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="F54">
+        <v>33.90365587321704</v>
+      </c>
+      <c r="H54">
+        <v>33.90365587321704</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55">
         <v>53</v>
       </c>
-      <c r="C55">
-        <v>37.87358136921825</v>
-      </c>
-      <c r="D55">
-        <v>103.2942633996571</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="F55">
+        <v>35.97852356405601</v>
+      </c>
+      <c r="H55">
+        <v>35.97852356405601</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56">
         <v>54</v>
       </c>
-      <c r="C56">
-        <v>40.47221951568521</v>
-      </c>
-      <c r="D56">
-        <v>103.3299993388778</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="F56">
+        <v>38.03186819976718</v>
+      </c>
+      <c r="H56">
+        <v>38.03186819976718</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57">
         <v>55</v>
       </c>
-      <c r="C57">
-        <v>43.07990036084898</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="F57">
+        <v>40.04824802908757</v>
+      </c>
+      <c r="H57">
+        <v>40.04824802908757</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58">
         <v>56</v>
       </c>
-      <c r="C58">
-        <v>45.67621825289194</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="F58">
+        <v>42.01333679291334</v>
+      </c>
+      <c r="H58">
+        <v>42.01333679291334</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59">
         <v>57</v>
       </c>
-      <c r="C59">
-        <v>48.24112085234183</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="F59">
+        <v>43.91430556098586</v>
+      </c>
+      <c r="H59">
+        <v>43.91430556098586</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60">
         <v>58</v>
       </c>
-      <c r="C60">
-        <v>50.75552067520922</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="F60">
+        <v>45.74011465934731</v>
+      </c>
+      <c r="H60">
+        <v>45.74011465934731</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61">
         <v>59</v>
       </c>
-      <c r="C61">
-        <v>53.20184452349041</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="F61">
+        <v>47.48170482291475</v>
+      </c>
+      <c r="H61">
+        <v>47.48170482291475</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62">
         <v>60</v>
       </c>
-      <c r="C62">
-        <v>55.56448856279952</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="F62">
+        <v>49.13208587270172</v>
+      </c>
+      <c r="H62">
+        <v>49.13208587270172</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63">
         <v>61</v>
       </c>
-      <c r="C63">
-        <v>57.83015664056865</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="F63">
+        <v>50.6863294388229</v>
+      </c>
+      <c r="H63">
+        <v>50.6863294388229</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64">
         <v>62</v>
       </c>
-      <c r="C64">
-        <v>59.98807083553761</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="F64">
+        <v>52.14147865880057</v>
+      </c>
+      <c r="H64">
+        <v>52.14147865880057</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65">
         <v>63</v>
       </c>
-      <c r="C65">
-        <v>62.03005456953715</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="F65">
+        <v>53.49639191722564</v>
+      </c>
+      <c r="H65">
+        <v>53.49639191722564</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66">
         <v>64</v>
       </c>
-      <c r="C66">
-        <v>63.95049848495015</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="F66">
+        <v>54.75153950743083</v>
+      </c>
+      <c r="H66">
+        <v>54.75153950743083</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67">
         <v>65</v>
       </c>
-      <c r="C67">
-        <v>65.74622671525755</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="F67">
+        <v>55.90877186598765</v>
+      </c>
+      <c r="H67">
+        <v>55.90877186598765</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68">
         <v>66</v>
       </c>
-      <c r="C68">
-        <v>67.41628569625472</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="F68">
+        <v>56.97107623908169</v>
+      </c>
+      <c r="H68">
+        <v>56.97107623908169</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69">
         <v>67</v>
       </c>
-      <c r="C69">
-        <v>68.96167932271595</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="F69">
+        <v>57.94233584678562</v>
+      </c>
+      <c r="H69">
+        <v>57.94233584678562</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70">
         <v>68</v>
       </c>
-      <c r="C70">
-        <v>70.38507346921959</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="F70">
+        <v>58.82710235135308</v>
+      </c>
+      <c r="H70">
+        <v>58.82710235135308</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71">
         <v>69</v>
       </c>
-      <c r="C71">
-        <v>71.69049030456772</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="F71">
+        <v>59.63038914881834</v>
+      </c>
+      <c r="H71">
+        <v>59.63038914881834</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72">
         <v>70</v>
       </c>
-      <c r="C72">
-        <v>72.88300914198715</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="F72">
+        <v>60.35749000362046</v>
+      </c>
+      <c r="H72">
+        <v>60.35749000362046</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73">
         <v>71</v>
       </c>
-      <c r="C73">
-        <v>73.96848643105658</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="F73">
+        <v>61.01382502093126</v>
+      </c>
+      <c r="H73">
+        <v>61.01382502093126</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74">
         <v>72</v>
       </c>
-      <c r="C74">
-        <v>74.95330342997534</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="F74">
+        <v>61.60481397934497</v>
+      </c>
+      <c r="H74">
+        <v>61.60481397934497</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75">
         <v>73</v>
       </c>
-      <c r="C75">
-        <v>75.84414645554362</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="F75">
+        <v>62.13577562468907</v>
+      </c>
+      <c r="H75">
+        <v>62.13577562468907</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76">
         <v>74</v>
       </c>
-      <c r="C76">
-        <v>76.64782159457832</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="F76">
+        <v>62.61185059830186</v>
+      </c>
+      <c r="H76">
+        <v>62.61185059830186</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77">
         <v>75</v>
       </c>
-      <c r="C77">
-        <v>77.37110344675642</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
+      <c r="F77">
+        <v>63.0379451567828</v>
+      </c>
+      <c r="H77">
+        <v>63.0379451567828</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78">
         <v>76</v>
       </c>
-      <c r="C78">
-        <v>78.02061583355226</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
+      <c r="F78">
+        <v>63.41869264280763</v>
+      </c>
+      <c r="H78">
+        <v>63.41869264280763</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79">
         <v>77</v>
       </c>
-      <c r="C79">
-        <v>78.60274137098497</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="F79">
+        <v>63.75842969999403</v>
+      </c>
+      <c r="H79">
+        <v>63.75842969999403</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80" s="1">
         <v>78</v>
       </c>
       <c r="B80">
         <v>78</v>
       </c>
-      <c r="C80">
-        <v>79.12355625651979</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="F80">
+        <v>64.06118441223164</v>
+      </c>
+      <c r="H80">
+        <v>64.06118441223164</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81">
         <v>79</v>
       </c>
-      <c r="C81">
-        <v>79.5887864471789</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
+      <c r="F81">
+        <v>64.33067382706462</v>
+      </c>
+      <c r="H81">
+        <v>64.33067382706462</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82">
         <v>80</v>
       </c>
-      <c r="C82">
-        <v>80.00378149887551</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="F82">
+        <v>64.57030864616202</v>
+      </c>
+      <c r="H82">
+        <v>64.57030864616202</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83">
         <v>81</v>
       </c>
-      <c r="C83">
-        <v>80.37350260384409</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
+      <c r="F83">
+        <v>64.78320319959656</v>
+      </c>
+      <c r="H83">
+        <v>64.78320319959656</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" s="1">
         <v>82</v>
       </c>
       <c r="B84">
         <v>82</v>
       </c>
-      <c r="C84">
-        <v>80.70252172995717</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="F84">
+        <v>64.97218914182822</v>
+      </c>
+      <c r="H84">
+        <v>64.97218914182822</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85">
         <v>83</v>
       </c>
-      <c r="C85">
-        <v>80.99502917717109</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
+      <c r="F85">
+        <v>65.13983160208322</v>
+      </c>
+      <c r="H85">
+        <v>65.13983160208322</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86">
         <v>84</v>
       </c>
-      <c r="C86">
-        <v>81.25484728310434</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="F86">
+        <v>65.2884467829905</v>
+      </c>
+      <c r="H86">
+        <v>65.2884467829905</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87">
         <v>85</v>
       </c>
-      <c r="C87">
-        <v>81.48544840606597</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="F87">
+        <v>65.42012022631582</v>
+      </c>
+      <c r="H87">
+        <v>65.42012022631582</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88">
         <v>86</v>
       </c>
-      <c r="C88">
-        <v>81.68997567443299</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="F88">
+        <v>65.5367251539558</v>
+      </c>
+      <c r="H88">
+        <v>65.5367251539558</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
       <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89">
         <v>87</v>
       </c>
-      <c r="C89">
-        <v>81.87126530855889</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
+      <c r="F89">
+        <v>65.63994044845717</v>
+      </c>
+      <c r="H89">
+        <v>65.63994044845717</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90">
         <v>88</v>
       </c>
-      <c r="C90">
-        <v>82.03186959318634</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
+      <c r="F90">
+        <v>65.73126796367468</v>
+      </c>
+      <c r="H90">
+        <v>65.73126796367468</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91">
         <v>89</v>
       </c>
-      <c r="C91">
-        <v>82.17407980596072</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
+      <c r="F91">
+        <v>65.81204895666058</v>
+      </c>
+      <c r="H91">
+        <v>65.81204895666058</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92">
         <v>90</v>
       </c>
-      <c r="C92">
-        <v>82.29994859452088</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
+      <c r="F92">
+        <v>65.88347951038752</v>
+      </c>
+      <c r="H92">
+        <v>65.88347951038752</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
       <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93">
         <v>91</v>
       </c>
-      <c r="C93">
-        <v>82.41131144530128</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="F93">
+        <v>65.94662487712924</v>
+      </c>
+      <c r="H93">
+        <v>65.94662487712924</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
       <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94">
         <v>92</v>
       </c>
-      <c r="C94">
-        <v>82.50980700651611</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="F94">
+        <v>66.0024327175764</v>
+      </c>
+      <c r="H94">
+        <v>66.0024327175764</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95">
         <v>93</v>
       </c>
-      <c r="C95">
-        <v>82.59689612066968</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="F95">
+        <v>66.05174524395639</v>
+      </c>
+      <c r="H95">
+        <v>66.05174524395639</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
       <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96">
         <v>94</v>
       </c>
-      <c r="C96">
-        <v>82.67387949286167</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="F96">
+        <v>66.09531029903748</v>
+      </c>
+      <c r="H96">
+        <v>66.09531029903748</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97">
         <v>95</v>
       </c>
-      <c r="C97">
-        <v>82.74191397418569</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="F97">
+        <v>66.1337914190064</v>
+      </c>
+      <c r="H97">
+        <v>66.1337914190064</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98" s="1">
         <v>96</v>
       </c>
       <c r="B98">
         <v>96</v>
       </c>
-      <c r="C98">
-        <v>82.80202747817343</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
+      <c r="F98">
+        <v>66.16777693852835</v>
+      </c>
+      <c r="H98">
+        <v>66.16777693852835</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
       <c r="A99" s="1">
         <v>97</v>
       </c>
       <c r="B99">
         <v>97</v>
       </c>
-      <c r="C99">
-        <v>82.85513257551078</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="F99">
+        <v>66.19778820221964</v>
+      </c>
+      <c r="H99">
+        <v>66.19778820221964</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100">
         <v>98</v>
       </c>
-      <c r="C100">
-        <v>82.90203883064314</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
+      <c r="F100">
+        <v>66.2242869494021</v>
+      </c>
+      <c r="H100">
+        <v>66.2242869494021</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
       <c r="A101" s="1">
         <v>99</v>
       </c>
       <c r="B101">
         <v>99</v>
       </c>
-      <c r="C101">
-        <v>82.94346395544497</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
+      <c r="F101">
+        <v>66.24768193924737</v>
+      </c>
+      <c r="H101">
+        <v>66.24768193924737</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
       <c r="A102" s="1">
         <v>100</v>
       </c>
       <c r="B102">
         <v>100</v>
       </c>
-      <c r="C102">
-        <v>82.98004386151705</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
+      <c r="F102">
+        <v>66.26833488195321</v>
+      </c>
+      <c r="H102">
+        <v>66.26833488195321</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
       <c r="A103" s="1">
         <v>101</v>
       </c>
       <c r="B103">
         <v>101</v>
       </c>
-      <c r="C103">
-        <v>83.0123416952197</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
+      <c r="F103">
+        <v>66.28656573895681</v>
+      </c>
+      <c r="H103">
+        <v>66.28656573895681</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
       <c r="A104" s="1">
         <v>102</v>
       </c>
       <c r="B104">
         <v>102</v>
       </c>
-      <c r="C104">
-        <v>83.04085593930225</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
+      <c r="F104">
+        <v>66.30265745179165</v>
+      </c>
+      <c r="H104">
+        <v>66.30265745179165</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
       <c r="A105" s="1">
         <v>103</v>
       </c>
       <c r="B105">
         <v>103</v>
       </c>
-      <c r="C105">
-        <v>83.06602766276961</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" s="1">
-        <v>104</v>
-      </c>
-      <c r="B106">
-        <v>104</v>
-      </c>
-      <c r="C106">
-        <v>83.08824699706773</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="1">
-        <v>105</v>
-      </c>
-      <c r="B107">
-        <v>105</v>
-      </c>
-      <c r="C107">
-        <v>83.10785891225352</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" s="1">
-        <v>106</v>
-      </c>
-      <c r="B108">
-        <v>106</v>
-      </c>
-      <c r="C108">
-        <v>83.12516836190736</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" s="1">
-        <v>107</v>
-      </c>
-      <c r="B109">
-        <v>107</v>
-      </c>
-      <c r="C109">
-        <v>83.14044486041104</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" s="1">
-        <v>108</v>
-      </c>
-      <c r="B110">
-        <v>108</v>
-      </c>
-      <c r="C110">
-        <v>83.15392655105092</v>
+      <c r="F105">
+        <v>66.31686015534662</v>
+      </c>
+      <c r="H105">
+        <v>66.31686015534662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first version of loading bar
</commit_message>
<xml_diff>
--- a/Strain_characterization.xlsx
+++ b/Strain_characterization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rwthaachende-my.sharepoint.com/personal/iris_broderius_rwth-aachen_de/Documents/Master/HiWi_Programmieren/GitLab/backup/aktuell_pushen_neu_2/biolabsim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="114_{BC9E0F97-1F1D-42EB-A8EC-644D3E15F2E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CAEE3E86-7404-46B5-9F46-04BECE4E1D1B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{BC86C3C7-D2F8-4630-88A7-CEAD3CD38991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <t>time</t>
   </si>
   <si>
-    <t>exp.1 biomass conc. at 10 °C</t>
+    <t>exp.1 biomass conc. at 20 °C</t>
   </si>
   <si>
     <t>exp.2 biomass conc. at 30 °C</t>
@@ -34,10 +34,10 @@
     <t>exp.3 biomass conc. at 32 °C</t>
   </si>
   <si>
-    <t>exp.4 biomass conc. at 38 °C</t>
+    <t>exp.4 biomass conc. at 35 °C</t>
   </si>
   <si>
-    <t>exp.5 biomass conc. at 35 °C</t>
+    <t>exp.5 biomass conc. at 38 °C</t>
   </si>
   <si>
     <t>exp.6 biomass conc. at 38 °C</t>
@@ -405,13 +405,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -444,22 +440,22 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>9.0712345965655194E-2</v>
+        <v>0.1015506491628967</v>
       </c>
       <c r="D2">
-        <v>0.1084792274211324</v>
+        <v>0.1051984933108476</v>
       </c>
       <c r="E2">
-        <v>0.1032578756458969</v>
+        <v>9.1931026983094841E-2</v>
       </c>
       <c r="F2">
-        <v>9.2119287123700114E-2</v>
+        <v>8.8804429585872577E-2</v>
       </c>
       <c r="G2">
-        <v>0.1035427211771144</v>
+        <v>0.1074895481366971</v>
       </c>
       <c r="H2">
-        <v>9.8319210160625059E-2</v>
+        <v>0.1154675389783444</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -470,22 +466,22 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>9.9491623519079891E-2</v>
+        <v>0.1651468423085975</v>
       </c>
       <c r="D3">
-        <v>0.22396940625689241</v>
+        <v>0.2172806702095795</v>
       </c>
       <c r="E3">
-        <v>0.25947041076581279</v>
+        <v>0.14950292235051149</v>
       </c>
       <c r="F3">
-        <v>0.190192191928204</v>
+        <v>0.1082203533419992</v>
       </c>
       <c r="G3">
-        <v>0.27542460998074902</v>
+        <v>0.1136910449598084</v>
       </c>
       <c r="H3">
-        <v>0.2029927355385284</v>
+        <v>0.1221293176215668</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -496,22 +492,22 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.1026616469949853</v>
+        <v>0.26849038078730458</v>
       </c>
       <c r="D4">
-        <v>0.46182502262718322</v>
+        <v>0.4483932484679749</v>
       </c>
       <c r="E4">
-        <v>0.65033310505341702</v>
+        <v>0.2430570030258096</v>
       </c>
       <c r="F4">
-        <v>0.3921763905558121</v>
+        <v>0.13187653480681019</v>
       </c>
       <c r="G4">
-        <v>0.73036812682534258</v>
+        <v>0.1202500271828644</v>
       </c>
       <c r="H4">
-        <v>0.41857111759142213</v>
+        <v>0.12917511461883249</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -522,22 +518,22 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0.1053987096519131</v>
+        <v>0.43629221166188492</v>
       </c>
       <c r="D5">
-        <v>0.94979261647860158</v>
+        <v>0.92369308036829656</v>
       </c>
       <c r="E5">
-        <v>1.6195801851642251</v>
+        <v>0.39496341395577522</v>
       </c>
       <c r="F5">
-        <v>0.80655274586070913</v>
+        <v>0.16069668988949601</v>
       </c>
       <c r="G5">
-        <v>1.9210701121392759</v>
+        <v>0.12718706603702609</v>
       </c>
       <c r="H5">
-        <v>0.86083632865528714</v>
+        <v>0.1366270280203899</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -548,22 +544,22 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>0.10602704212654571</v>
+        <v>0.70841192895187965</v>
       </c>
       <c r="D6">
-        <v>1.94292450576522</v>
+        <v>1.8959128419223501</v>
       </c>
       <c r="E6">
-        <v>3.9705223963178149</v>
+        <v>0.6413059561160942</v>
       </c>
       <c r="F6">
-        <v>1.6499086936840861</v>
+        <v>0.195804638024102</v>
       </c>
       <c r="G6">
-        <v>4.9478872622154837</v>
+        <v>0.1345239122342389</v>
       </c>
       <c r="H6">
-        <v>1.760952832628176</v>
+        <v>0.14450842289961499</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -574,22 +570,22 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>9.7676921741675068E-2</v>
+        <v>1.1487960735495291</v>
       </c>
       <c r="D7">
-        <v>3.9317948096305049</v>
+        <v>3.862772431267937</v>
       </c>
       <c r="E7">
-        <v>9.3794902380808889</v>
+        <v>1.0399736851129999</v>
       </c>
       <c r="F7">
-        <v>3.3388340200261122</v>
+        <v>0.23856710652549229</v>
       </c>
       <c r="G7">
-        <v>12.10399342479492</v>
+        <v>0.1422835630868465</v>
       </c>
       <c r="H7">
-        <v>3.563548242243566</v>
+        <v>0.1528440034543157</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -600,22 +596,22 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>9.8812453466384134E-2</v>
+        <v>1.859127859352341</v>
       </c>
       <c r="D8">
-        <v>7.7889468439118827</v>
+        <v>7.7545690583751199</v>
       </c>
       <c r="E8">
-        <v>20.443783985329478</v>
+        <v>1.6830176351604149</v>
       </c>
       <c r="F8">
-        <v>6.6142822710201266</v>
+        <v>0.29064542758033851</v>
       </c>
       <c r="G8">
-        <v>26.468552203333779</v>
+        <v>0.1504903333863713</v>
       </c>
       <c r="H8">
-        <v>7.0594446502052284</v>
+        <v>0.1616598891462119</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -625,20 +621,23 @@
       <c r="B9">
         <v>7</v>
       </c>
+      <c r="C9">
+        <v>2.998766381680086</v>
+      </c>
       <c r="D9">
-        <v>14.824351953502861</v>
+        <v>15.12801301998115</v>
       </c>
       <c r="E9">
-        <v>38.474510752847287</v>
+        <v>2.714701239457503</v>
       </c>
       <c r="F9">
-        <v>12.58866574266813</v>
+        <v>0.35405784683660763</v>
       </c>
       <c r="G9">
-        <v>47.718292934548877</v>
+        <v>0.15916993024479861</v>
       </c>
       <c r="H9">
-        <v>13.435923262554381</v>
+        <v>0.17098369509702149</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -648,20 +647,23 @@
       <c r="B10">
         <v>8</v>
       </c>
+      <c r="C10">
+        <v>4.8115706179767717</v>
+      </c>
       <c r="D10">
-        <v>26.32941768027796</v>
+        <v>28.014419363922212</v>
       </c>
       <c r="E10">
-        <v>59.226790432962368</v>
+        <v>4.3557833648384294</v>
       </c>
       <c r="F10">
-        <v>22.358632567260141</v>
+        <v>0.43125443116838341</v>
       </c>
       <c r="G10">
-        <v>68.291040948594897</v>
+        <v>0.16834953211182899</v>
       </c>
       <c r="H10">
-        <v>23.863440142917469</v>
+        <v>0.18084461697045839</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -671,20 +673,23 @@
       <c r="B11">
         <v>9</v>
       </c>
+      <c r="C11">
+        <v>7.656221193461394</v>
+      </c>
       <c r="D11">
-        <v>42.15734917338974</v>
+        <v>47.650505189708277</v>
       </c>
       <c r="E11">
-        <v>75.37932194445095</v>
+        <v>6.9309677774251366</v>
       </c>
       <c r="F11">
-        <v>35.799526279821571</v>
+        <v>0.52520684052074496</v>
       </c>
       <c r="G11">
-        <v>81.471054988628183</v>
+        <v>0.17805787219209121</v>
       </c>
       <c r="H11">
-        <v>38.208949047012773</v>
+        <v>0.19127352058076211</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -694,20 +699,23 @@
       <c r="B12">
         <v>10</v>
       </c>
+      <c r="C12">
+        <v>12.026157885785871</v>
+      </c>
       <c r="D12">
-        <v>59.444985250219887</v>
+        <v>72.097968586921439</v>
       </c>
       <c r="E12">
-        <v>84.538880789826479</v>
+        <v>10.8869520206384</v>
       </c>
       <c r="F12">
-        <v>50.479983997953518</v>
+        <v>0.63951549408964903</v>
       </c>
       <c r="G12">
-        <v>87.831816775257167</v>
+        <v>0.1883253264972316</v>
       </c>
       <c r="H12">
-        <v>53.877448583977163</v>
+        <v>0.20230303648010761</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -717,20 +725,23 @@
       <c r="B13">
         <v>11</v>
       </c>
+      <c r="C13">
+        <v>18.524748409330421</v>
+      </c>
       <c r="D13">
-        <v>74.156146279389844</v>
+        <v>95.900609341232638</v>
       </c>
       <c r="E13">
-        <v>88.826959950099862</v>
+        <v>16.769948394336978</v>
       </c>
       <c r="F13">
-        <v>62.972529335763483</v>
+        <v>0.77853687961233065</v>
       </c>
       <c r="G13">
-        <v>90.482611155780461</v>
+        <v>0.19918400677911671</v>
       </c>
       <c r="H13">
-        <v>67.210782230599264</v>
+        <v>0.21396765978941229</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -740,20 +751,23 @@
       <c r="B14">
         <v>12</v>
       </c>
+      <c r="C14">
+        <v>27.7367506581447</v>
+      </c>
       <c r="D14">
-        <v>84.241609808176491</v>
+        <v>114.12836455875301</v>
       </c>
       <c r="E14">
-        <v>90.653746141780218</v>
+        <v>25.109322236700311</v>
       </c>
       <c r="F14">
-        <v>71.536986630219786</v>
+        <v>0.94753387048071791</v>
       </c>
       <c r="G14">
-        <v>91.519043053431119</v>
+        <v>0.21066785860210141</v>
       </c>
       <c r="H14">
-        <v>76.351654928784839</v>
+        <v>0.22630385554963359</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -763,20 +777,23 @@
       <c r="B15">
         <v>13</v>
       </c>
+      <c r="C15">
+        <v>39.945685522408638</v>
+      </c>
       <c r="D15">
-        <v>90.174552987210006</v>
+        <v>125.6850391881956</v>
       </c>
       <c r="E15">
-        <v>91.400516785704241</v>
+        <v>36.161737260075427</v>
       </c>
       <c r="F15">
-        <v>76.575172365782265</v>
+        <v>1.152851842875434</v>
       </c>
       <c r="G15">
-        <v>91.914102929757618</v>
+        <v>0.22281276482441331</v>
       </c>
       <c r="H15">
-        <v>81.728926699221589</v>
+        <v>0.23935016988365371</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -786,20 +803,23 @@
       <c r="B16">
         <v>14</v>
       </c>
+      <c r="C16">
+        <v>54.760479569503417</v>
+      </c>
       <c r="D16">
-        <v>93.355230719545219</v>
+        <v>132.15905407836661</v>
       </c>
       <c r="E16">
-        <v>91.70061914820667</v>
+        <v>49.573165375200382</v>
       </c>
       <c r="F16">
-        <v>79.276166576733544</v>
+        <v>1.4021229960167521</v>
       </c>
       <c r="G16">
-        <v>92.063225288225894</v>
+        <v>0.23565665477117889</v>
       </c>
       <c r="H16">
-        <v>84.611706470547333</v>
+        <v>0.25314734727224669</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -809,17 +829,23 @@
       <c r="B17">
         <v>15</v>
       </c>
+      <c r="C17">
+        <v>70.928299747631272</v>
+      </c>
       <c r="D17">
-        <v>94.975870265697154</v>
+        <v>135.53646372517181</v>
       </c>
       <c r="E17">
-        <v>91.820391221257893</v>
+        <v>64.209451064217433</v>
       </c>
       <c r="F17">
-        <v>80.652394664129673</v>
+        <v>1.7045003872810831</v>
+      </c>
+      <c r="G17">
+        <v>0.2492396193944495</v>
       </c>
       <c r="H17">
-        <v>86.080559115617817</v>
+        <v>0.26773845426140641</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -829,14 +855,23 @@
       <c r="B18">
         <v>16</v>
       </c>
+      <c r="C18">
+        <v>86.652630023596515</v>
+      </c>
       <c r="D18">
-        <v>95.780250189836579</v>
+        <v>137.233077943236</v>
+      </c>
+      <c r="E18">
+        <v>78.444257466804316</v>
       </c>
       <c r="F18">
-        <v>81.335464657803911</v>
+        <v>2.070921539384297</v>
+      </c>
+      <c r="G18">
+        <v>0.26360403272875849</v>
       </c>
       <c r="H18">
-        <v>86.80960190740899</v>
+        <v>0.28316900993246619</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -846,14 +881,23 @@
       <c r="B19">
         <v>17</v>
       </c>
+      <c r="C19">
+        <v>100.3222358549622</v>
+      </c>
       <c r="D19">
-        <v>96.174293925702614</v>
+        <v>138.06918365271989</v>
+      </c>
+      <c r="E19">
+        <v>90.818977991886797</v>
       </c>
       <c r="F19">
-        <v>81.670081974929701</v>
+        <v>2.514398704784762</v>
+      </c>
+      <c r="G19">
+        <v>0.27879467996422358</v>
       </c>
       <c r="H19">
-        <v>87.166740041594693</v>
+        <v>0.29948712348092688</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -863,14 +907,23 @@
       <c r="B20">
         <v>18</v>
       </c>
+      <c r="C20">
+        <v>111.0935658426805</v>
+      </c>
       <c r="D20">
-        <v>96.366085780853481</v>
+        <v>138.47733248116529</v>
+      </c>
+      <c r="E20">
+        <v>100.569968614865</v>
       </c>
       <c r="F20">
-        <v>81.832949368002488</v>
+        <v>3.0503285221598451</v>
+      </c>
+      <c r="G20">
+        <v>0.29485889247297342</v>
       </c>
       <c r="H20">
-        <v>87.340568931806729</v>
+        <v>0.31674363926468979</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -880,14 +933,23 @@
       <c r="B21">
         <v>19</v>
       </c>
+      <c r="C21">
+        <v>118.9425906772038</v>
+      </c>
       <c r="D21">
-        <v>96.459143420894165</v>
+        <v>138.67564927162741</v>
+      </c>
+      <c r="E21">
+        <v>107.6754762586032</v>
       </c>
       <c r="F21">
-        <v>81.91197282406641</v>
+        <v>3.6968073063556379</v>
+      </c>
+      <c r="G21">
+        <v>0.31184669013867677</v>
       </c>
       <c r="H21">
-        <v>87.424910919537638</v>
+        <v>0.33499228969743988</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -897,6 +959,24 @@
       <c r="B22">
         <v>20</v>
       </c>
+      <c r="C22">
+        <v>124.3420594493732</v>
+      </c>
+      <c r="D22">
+        <v>138.7717926713112</v>
+      </c>
+      <c r="E22">
+        <v>112.5634677532951</v>
+      </c>
+      <c r="F22">
+        <v>4.4749289438171642</v>
+      </c>
+      <c r="G22">
+        <v>0.32981093135315348</v>
+      </c>
+      <c r="H22">
+        <v>0.3542898563781654</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -905,6 +985,21 @@
       <c r="B23">
         <v>21</v>
       </c>
+      <c r="C23">
+        <v>127.9109019542371</v>
+      </c>
+      <c r="E23">
+        <v>115.794243325067</v>
+      </c>
+      <c r="F23">
+        <v>5.4090297198345798</v>
+      </c>
+      <c r="G23">
+        <v>0.34880747105835741</v>
+      </c>
+      <c r="H23">
+        <v>0.37469633986319029</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -913,6 +1008,21 @@
       <c r="B24">
         <v>22</v>
       </c>
+      <c r="C24">
+        <v>130.2078580944777</v>
+      </c>
+      <c r="E24">
+        <v>117.8736149356681</v>
+      </c>
+      <c r="F24">
+        <v>6.5268280221469492</v>
+      </c>
+      <c r="G24">
+        <v>0.3688953272264221</v>
+      </c>
+      <c r="H24">
+        <v>0.39627513850254842</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -921,6 +1031,21 @@
       <c r="B25">
         <v>23</v>
       </c>
+      <c r="C25">
+        <v>131.661001504382</v>
+      </c>
+      <c r="E25">
+        <v>119.18910594559679</v>
+      </c>
+      <c r="F25">
+        <v>7.8593869984750633</v>
+      </c>
+      <c r="G25">
+        <v>0.39013685618481692</v>
+      </c>
+      <c r="H25">
+        <v>0.41909323677796317</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -929,6 +1054,21 @@
       <c r="B26">
         <v>24</v>
       </c>
+      <c r="C26">
+        <v>132.57033632393211</v>
+      </c>
+      <c r="E26">
+        <v>120.0123019027062</v>
+      </c>
+      <c r="F26">
+        <v>9.4408063380027052</v>
+      </c>
+      <c r="G26">
+        <v>0.4125979372079126</v>
+      </c>
+      <c r="H26">
+        <v>0.44322140359499917</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
@@ -937,6 +1077,21 @@
       <c r="B27">
         <v>25</v>
       </c>
+      <c r="C27">
+        <v>133.1354901726844</v>
+      </c>
+      <c r="E27">
+        <v>120.5239202345192</v>
+      </c>
+      <c r="F27">
+        <v>11.307528839910431</v>
+      </c>
+      <c r="G27">
+        <v>0.43634816681028238</v>
+      </c>
+      <c r="H27">
+        <v>0.46873440099702313</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -945,6 +1100,21 @@
       <c r="B28">
         <v>26</v>
       </c>
+      <c r="C28">
+        <v>133.48524181722459</v>
+      </c>
+      <c r="E28">
+        <v>120.8405408384902</v>
+      </c>
+      <c r="F28">
+        <v>13.497134676505709</v>
+      </c>
+      <c r="G28">
+        <v>0.46146106319072611</v>
+      </c>
+      <c r="H28">
+        <v>0.49571120378328409</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -953,6 +1123,21 @@
       <c r="B29">
         <v>27</v>
       </c>
+      <c r="C29">
+        <v>133.70111920167199</v>
+      </c>
+      <c r="E29">
+        <v>121.03596873401101</v>
+      </c>
+      <c r="F29">
+        <v>16.046501194759301</v>
+      </c>
+      <c r="G29">
+        <v>0.48801428128916691</v>
+      </c>
+      <c r="H29">
+        <v>0.5242352305275686</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -961,6 +1146,21 @@
       <c r="B30">
         <v>28</v>
       </c>
+      <c r="C30">
+        <v>133.8341484128949</v>
+      </c>
+      <c r="E30">
+        <v>121.1563964428172</v>
+      </c>
+      <c r="F30">
+        <v>18.989242009754872</v>
+      </c>
+      <c r="G30">
+        <v>0.5160898389310602</v>
+      </c>
+      <c r="H30">
+        <v>0.55439458650729023</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -969,6 +1169,21 @@
       <c r="B31">
         <v>29</v>
       </c>
+      <c r="C31">
+        <v>133.9160421631839</v>
+      </c>
+      <c r="E31">
+        <v>121.2305326165357</v>
+      </c>
+      <c r="F31">
+        <v>22.35242040177339</v>
+      </c>
+      <c r="G31">
+        <v>0.54577435454555723</v>
+      </c>
+      <c r="H31">
+        <v>0.58628231906535488</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -977,341 +1192,734 @@
       <c r="B32">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>133.96642538905891</v>
+      </c>
+      <c r="E32">
+        <v>121.2761431737857</v>
+      </c>
+      <c r="F32">
+        <v>26.152668707011902</v>
+      </c>
+      <c r="G32">
+        <v>0.57715929695419799</v>
+      </c>
+      <c r="H32">
+        <v>0.61999668593844059</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>30.392034345017588</v>
+      </c>
+      <c r="G33">
+        <v>0.61034124773607246</v>
+      </c>
+      <c r="H33">
+        <v>0.65564143709518619</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>35.054087444468877</v>
+      </c>
+      <c r="G34">
+        <v>0.64542217668293422</v>
+      </c>
+      <c r="H34">
+        <v>0.69332611063588145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>40.101007366092297</v>
+      </c>
+      <c r="G35">
+        <v>0.68250973086333344</v>
+      </c>
+      <c r="H35">
+        <v>0.73316634331125441</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>45.472433835414392</v>
+      </c>
+      <c r="G36">
+        <v>0.72171753781809866</v>
+      </c>
+      <c r="H36">
+        <v>0.77528419622144962</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>51.086741990284033</v>
+      </c>
+      <c r="G37">
+        <v>0.76316552341003097</v>
+      </c>
+      <c r="H37">
+        <v>0.81980849625687213</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>56.845042548995579</v>
+      </c>
+      <c r="G38">
+        <v>0.80698024484801245</v>
+      </c>
+      <c r="H38">
+        <v>0.86687519383970635</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>62.63766714917211</v>
+      </c>
+      <c r="G39">
+        <v>0.85329523939936713</v>
+      </c>
+      <c r="H39">
+        <v>0.91662773751808646</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>68.35231830485742</v>
+      </c>
+      <c r="G40">
+        <v>0.90225138929367921</v>
+      </c>
+      <c r="H40">
+        <v>0.96921746595347147</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>73.882637902572711</v>
+      </c>
+      <c r="G41">
+        <v>0.95399730330569887</v>
+      </c>
+      <c r="H41">
+        <v>1.024804017825049</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>79.135837090935013</v>
+      </c>
+      <c r="G42">
+        <v>1.0086897154837839</v>
+      </c>
+      <c r="H42">
+        <v>1.083555760152233</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>84.038277276080279</v>
+      </c>
+      <c r="G43">
+        <v>1.066493901462727</v>
+      </c>
+      <c r="H43">
+        <v>1.1456502355066831</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>88.538401110019421</v>
+      </c>
+      <c r="G44">
+        <v>1.1275841127649271</v>
+      </c>
+      <c r="H44">
+        <v>1.211274628547776</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>92.606999509312175</v>
+      </c>
+      <c r="G45">
+        <v>1.1921440294507031</v>
+      </c>
+      <c r="H45">
+        <v>1.2806262522691201</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>96.235282575423668</v>
+      </c>
+      <c r="G46">
+        <v>1.2603672314261649</v>
+      </c>
+      <c r="H46">
+        <v>1.353913054287406</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>99.431490206401719</v>
+      </c>
+      <c r="G47">
+        <v>1.3324576886540831</v>
+      </c>
+      <c r="H47">
+        <v>1.4313541434372581</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>102.21682056905181</v>
+      </c>
+      <c r="G48">
+        <v>1.408630270438636</v>
+      </c>
+      <c r="H48">
+        <v>1.51318033685565</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>104.621331155782</v>
+      </c>
+      <c r="G49">
+        <v>1.4891112738671159</v>
+      </c>
+      <c r="H49">
+        <v>1.599634727645127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>106.68026357735459</v>
+      </c>
+      <c r="G50">
+        <v>1.574138971389337</v>
+      </c>
+      <c r="H50">
+        <v>1.6909732730951481</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>108.4310337380951</v>
+      </c>
+      <c r="G51">
+        <v>1.6639641773968299</v>
+      </c>
+      <c r="H51">
+        <v>1.787465403313407</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>109.9109588506287</v>
+      </c>
+      <c r="G52">
+        <v>1.758850833527307</v>
+      </c>
+      <c r="H52">
+        <v>1.8893946499722281</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>111.1556783175167</v>
+      </c>
+      <c r="G53">
+        <v>1.8590766122632549</v>
+      </c>
+      <c r="H53">
+        <v>1.997059294706901</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>112.19816357192749</v>
+      </c>
+      <c r="G54">
+        <v>1.964933538215063</v>
+      </c>
+      <c r="H54">
+        <v>2.1107730365111159</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>113.0681898980409</v>
+      </c>
+      <c r="G55">
+        <v>2.076728626276366</v>
+      </c>
+      <c r="H55">
+        <v>2.2308656772568889</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>113.7921466499793</v>
+      </c>
+      <c r="G56">
+        <v>2.194784535610276</v>
+      </c>
+      <c r="H56">
+        <v>2.357683824220365</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>114.3930790498494</v>
+      </c>
+      <c r="G57">
+        <v>2.3194402381671968</v>
+      </c>
+      <c r="H57">
+        <v>2.491591608217739</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>114.89087637535479</v>
+      </c>
+      <c r="G58">
+        <v>2.451051700145582</v>
+      </c>
+      <c r="H58">
+        <v>2.6329714156447812</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>115.302542736882</v>
+      </c>
+      <c r="G59">
+        <v>2.589992574483599</v>
+      </c>
+      <c r="H59">
+        <v>2.7822246323659812</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>115.64250523923459</v>
+      </c>
+      <c r="G60">
+        <v>2.736654902109513</v>
+      </c>
+      <c r="H60">
+        <v>2.9397723970124892</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>115.9229292304255</v>
+      </c>
+      <c r="G61">
+        <v>2.891449819278801</v>
+      </c>
+      <c r="H61">
+        <v>3.106056360818569</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>116.154021603682</v>
+      </c>
+      <c r="G62">
+        <v>3.054808267883975</v>
+      </c>
+      <c r="H62">
+        <v>3.2815394506513749</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>116.34431122676369</v>
+      </c>
+      <c r="G63">
+        <v>3.2271817051357869</v>
+      </c>
+      <c r="H63">
+        <v>3.4667066313654749</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>116.5009011555605</v>
+      </c>
+      <c r="G64">
+        <v>3.4090428084794371</v>
+      </c>
+      <c r="H64">
+        <v>3.6620656630387001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>116.62969096055799</v>
+      </c>
+      <c r="G65">
+        <v>3.6008861710239559</v>
+      </c>
+      <c r="H65">
+        <v>3.8681478480170481</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66">
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>116.7355697812454</v>
+      </c>
+      <c r="G66">
+        <v>3.8032289821247081</v>
+      </c>
+      <c r="H66">
+        <v>4.085508762010762</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>116.8225820431516</v>
+      </c>
+      <c r="G67">
+        <v>4.0166116870661641</v>
+      </c>
+      <c r="H67">
+        <v>4.3147289627394736</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68">
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>116.89406844074971</v>
+      </c>
+      <c r="G68">
+        <v>4.241598619042934</v>
+      </c>
+      <c r="H68">
+        <v>4.5564146688195466</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>116.9527850362842</v>
+      </c>
+      <c r="G69">
+        <v>4.4787785958306419</v>
+      </c>
+      <c r="H69">
+        <v>4.8111984007205253</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70">
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>117.0010033108186</v>
+      </c>
+      <c r="G70">
+        <v>4.7287654726744401</v>
+      </c>
+      <c r="H70">
+        <v>5.0797395746896177</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71">
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>117.04059383945081</v>
+      </c>
+      <c r="G71">
+        <v>4.9921986420020943</v>
+      </c>
+      <c r="H71">
+        <v>5.3627250395540376</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>117.0730960205094</v>
+      </c>
+      <c r="G72">
+        <v>5.2697434695927514</v>
+      </c>
+      <c r="H72">
+        <v>5.66086954526269</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73">
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>117.0997760152741</v>
+      </c>
+      <c r="G73">
+        <v>5.5620916558045037</v>
+      </c>
+      <c r="H73">
+        <v>5.9749161309244387</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74">
         <v>72</v>
+      </c>
+      <c r="F74">
+        <v>117.1216747789811</v>
+      </c>
+      <c r="G74">
+        <v>5.8699615093884354</v>
+      </c>
+      <c r="H74">
+        <v>6.3056364189449194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename AvailableExpress to TargetExpress, remove TempExp plot
</commit_message>
<xml_diff>
--- a/Strain_characterization.xlsx
+++ b/Strain_characterization.xlsx
@@ -435,22 +435,22 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.118646868120034</v>
+        <v>0.1005014384359282</v>
       </c>
       <c r="E2">
-        <v>0.100416833003408</v>
+        <v>0.08738153734997885</v>
       </c>
       <c r="F2">
-        <v>0.1032637044054066</v>
+        <v>0.103930871891134</v>
       </c>
       <c r="G2">
-        <v>0.09209714169955334</v>
+        <v>0.1193641773726557</v>
       </c>
       <c r="H2">
-        <v>0.0904976789397621</v>
+        <v>0.09750644845397141</v>
       </c>
       <c r="I2">
-        <v>0.1043948510115738</v>
+        <v>0.09629327895446765</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -461,22 +461,22 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.1358231842415622</v>
+        <v>0.1326650888701779</v>
       </c>
       <c r="E3">
-        <v>0.2725316321024404</v>
+        <v>0.2195534903288444</v>
       </c>
       <c r="F3">
-        <v>0.2595661055202136</v>
+        <v>0.2145634427616105</v>
       </c>
       <c r="G3">
-        <v>0.1687822917720807</v>
+        <v>0.1736337480131572</v>
       </c>
       <c r="H3">
-        <v>0.1194702609148403</v>
+        <v>0.1116178839334666</v>
       </c>
       <c r="I3">
-        <v>0.1378165742440796</v>
+        <v>0.110229140783303</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -487,22 +487,22 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>0.155483095716822</v>
+        <v>0.1751007530904355</v>
       </c>
       <c r="E4">
-        <v>0.7376617934579943</v>
+        <v>0.5501464593498983</v>
       </c>
       <c r="F4">
-        <v>0.6510817845306941</v>
+        <v>0.4423649824135962</v>
       </c>
       <c r="G4">
-        <v>0.3091229154305613</v>
+        <v>0.2525150590090808</v>
       </c>
       <c r="H4">
-        <v>0.1577034922910531</v>
+        <v>0.1277683804926976</v>
       </c>
       <c r="I4">
-        <v>0.1819210478612153</v>
+        <v>0.1261786938137915</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -513,22 +513,22 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>0.1779847872711686</v>
+        <v>0.2310731272545919</v>
       </c>
       <c r="E5">
-        <v>1.98221802957452</v>
+        <v>1.369216570155795</v>
       </c>
       <c r="F5">
-        <v>1.624595577515788</v>
+        <v>0.9094970926146908</v>
       </c>
       <c r="G5">
-        <v>0.5654967695820003</v>
+        <v>0.3671004909026367</v>
       </c>
       <c r="H5">
-        <v>0.2081463875160585</v>
+        <v>0.1462515869815051</v>
       </c>
       <c r="I5">
-        <v>0.240110148325461</v>
+        <v>0.1444319333340467</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -539,22 +539,22 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>0.2037378129836032</v>
+        <v>0.3048727759545362</v>
       </c>
       <c r="E6">
-        <v>5.225616106737893</v>
+        <v>3.35163288701035</v>
       </c>
       <c r="F6">
-        <v>4.001679719966655</v>
+        <v>1.859355599167888</v>
       </c>
       <c r="G6">
-        <v>1.032303311094829</v>
+        <v>0.5334048006170847</v>
       </c>
       <c r="H6">
-        <v>0.2746789009543175</v>
+        <v>0.1674031343264421</v>
       </c>
       <c r="I6">
-        <v>0.3168596507346422</v>
+        <v>0.1653203143703647</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -565,22 +565,22 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>0.2332103740653598</v>
+        <v>0.4021298202492091</v>
       </c>
       <c r="E7">
-        <v>13.12776209045076</v>
+        <v>7.889895738968978</v>
       </c>
       <c r="F7">
-        <v>9.557227189105479</v>
+        <v>3.758072672613569</v>
       </c>
       <c r="G7">
-        <v>1.877202914225348</v>
+        <v>0.774464422738091</v>
       </c>
       <c r="H7">
-        <v>0.3623997633199519</v>
+        <v>0.1916065424345351</v>
       </c>
       <c r="I7">
-        <v>0.4180512665258355</v>
+        <v>0.1892225850976346</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -591,22 +591,22 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>0.2669375999415681</v>
+        <v>0.5302171326749893</v>
       </c>
       <c r="E8">
-        <v>29.58736506431835</v>
+        <v>17.07525126971877</v>
       </c>
       <c r="F8">
-        <v>21.31140664705768</v>
+        <v>7.427160187544572</v>
       </c>
       <c r="G8">
-        <v>3.390024446047063</v>
+        <v>1.123238260862922</v>
       </c>
       <c r="H8">
-        <v>0.4779988412319327</v>
+        <v>0.2192999286385518</v>
       </c>
       <c r="I8">
-        <v>0.5514021839977555</v>
+        <v>0.216571411818526</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -617,22 +617,22 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <v>0.3055309622681081</v>
+        <v>0.6987637981743835</v>
       </c>
       <c r="E9">
-        <v>54.91830450103931</v>
+        <v>31.76845280092449</v>
       </c>
       <c r="F9">
-        <v>41.67291547042656</v>
+        <v>14.07494877620415</v>
       </c>
       <c r="G9">
-        <v>6.047174273878181</v>
+        <v>1.626511818244011</v>
       </c>
       <c r="H9">
-        <v>0.6302355083468215</v>
+        <v>0.2509836171937477</v>
       </c>
       <c r="I9">
-        <v>0.7270168999567808</v>
+        <v>0.2478608937833231</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -643,22 +643,22 @@
         <v>8</v>
       </c>
       <c r="D10">
-        <v>0.3496889655049257</v>
+        <v>0.9203007116220582</v>
       </c>
       <c r="E10">
-        <v>80.16761201160389</v>
+        <v>48.26986315428803</v>
       </c>
       <c r="F10">
-        <v>67.16794948392732</v>
+        <v>24.82371709769559</v>
       </c>
       <c r="G10">
-        <v>10.56028400550026</v>
+        <v>2.349935272621139</v>
       </c>
       <c r="H10">
-        <v>0.8305474298436756</v>
+        <v>0.2872287587243096</v>
       </c>
       <c r="I10">
-        <v>0.9580894914917024</v>
+        <v>0.2836550753937231</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -669,22 +669,22 @@
         <v>9</v>
       </c>
       <c r="D11">
-        <v>0.4002092722437788</v>
+        <v>1.211057974817014</v>
       </c>
       <c r="E11">
-        <v>96.48712684273711</v>
+        <v>60.82067797083769</v>
       </c>
       <c r="F11">
-        <v>88.73510321553071</v>
+        <v>39.36802113654208</v>
       </c>
       <c r="G11">
-        <v>17.80587485912468</v>
+        <v>3.384076988748477</v>
       </c>
       <c r="H11">
-        <v>1.093815297764373</v>
+        <v>0.3286870777724712</v>
       </c>
       <c r="I11">
-        <v>1.2617857870178</v>
+        <v>0.3245975724735185</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -695,22 +695,22 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>0.4580024363155369</v>
+        <v>1.591924975085801</v>
       </c>
       <c r="E12">
-        <v>104.2978096628945</v>
+        <v>67.82707255054829</v>
       </c>
       <c r="F12">
-        <v>101.7095257590957</v>
+        <v>54.94042338852611</v>
       </c>
       <c r="G12">
-        <v>28.44833934185827</v>
+        <v>4.850770380048016</v>
       </c>
       <c r="H12">
-        <v>1.439306129719827</v>
+        <v>0.3761018752752123</v>
       </c>
       <c r="I12">
-        <v>1.660331521564891</v>
+        <v>0.371422437853128</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -721,22 +721,22 @@
         <v>11</v>
       </c>
       <c r="D13">
-        <v>0.5241074312749351</v>
+        <v>2.089563388138862</v>
       </c>
       <c r="E13">
-        <v>107.4991373072398</v>
+        <v>71.08009451894706</v>
       </c>
       <c r="F13">
-        <v>107.9820111022372</v>
+        <v>67.94169701921535</v>
       </c>
       <c r="G13">
-        <v>42.20109344187937</v>
+        <v>6.907818689444817</v>
       </c>
       <c r="H13">
-        <v>1.891806833262987</v>
+        <v>0.4303204202511933</v>
       </c>
       <c r="I13">
-        <v>2.182319975660648</v>
+        <v>0.4249663988798906</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -747,22 +747,22 @@
         <v>12</v>
       </c>
       <c r="D14">
-        <v>0.5997091754511894</v>
+        <v>2.737622842449596</v>
       </c>
       <c r="E14">
-        <v>108.7268514728644</v>
+        <v>72.46074057310769</v>
       </c>
       <c r="F14">
-        <v>110.6940631468934</v>
+        <v>76.72523775733528</v>
       </c>
       <c r="G14">
-        <v>57.30608935574099</v>
+        <v>9.748070970487539</v>
       </c>
       <c r="H14">
-        <v>2.48293449141365</v>
+        <v>0.4923078703558668</v>
       </c>
       <c r="I14">
-        <v>2.864223473346322</v>
+        <v>0.4861826047744492</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -773,22 +773,22 @@
         <v>13</v>
       </c>
       <c r="D15">
-        <v>0.6861582663400831</v>
+        <v>3.577937616712386</v>
       </c>
       <c r="E15">
-        <v>109.1855877886717</v>
+        <v>73.02424469569515</v>
       </c>
       <c r="F15">
-        <v>111.8096971524905</v>
+        <v>81.8439069457235</v>
       </c>
       <c r="G15">
-        <v>71.20156944636749</v>
+        <v>13.58618621472903</v>
       </c>
       <c r="H15">
-        <v>3.252560668386479</v>
+        <v>0.5631628630826522</v>
       </c>
       <c r="I15">
-        <v>3.752036409777162</v>
+        <v>0.5561560238471159</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -799,22 +799,22 @@
         <v>14</v>
       </c>
       <c r="D16">
-        <v>0.784993145294925</v>
+        <v>4.661467776918208</v>
       </c>
       <c r="E16">
-        <v>109.3553229259626</v>
+        <v>73.25055321489647</v>
       </c>
       <c r="F16">
-        <v>112.2591818924887</v>
+        <v>84.573452585034</v>
       </c>
       <c r="G16">
-        <v>82.04918072467315</v>
+        <v>18.62455088748744</v>
       </c>
       <c r="H16">
-        <v>4.250200924991801</v>
+        <v>0.6441349166923989</v>
       </c>
       <c r="I16">
-        <v>4.902878145958981</v>
+        <v>0.6361206279259949</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -825,19 +825,22 @@
         <v>15</v>
       </c>
       <c r="D17">
-        <v>0.8979649163583185</v>
+        <v>6.048580022317476</v>
+      </c>
+      <c r="E17">
+        <v>73.34085065465324</v>
       </c>
       <c r="F17">
-        <v>112.4387574333035</v>
+        <v>85.96033482261579</v>
       </c>
       <c r="G17">
-        <v>89.48225642285931</v>
+        <v>24.99263011398891</v>
       </c>
       <c r="H17">
-        <v>5.536082785474666</v>
+        <v>0.7366437703956698</v>
       </c>
       <c r="I17">
-        <v>6.386224976687621</v>
+        <v>0.7274784919098541</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -848,19 +851,19 @@
         <v>16</v>
       </c>
       <c r="D18">
-        <v>1.027065038150029</v>
+        <v>7.808047797650645</v>
       </c>
       <c r="F18">
-        <v>112.5102585949471</v>
+        <v>86.647719971782</v>
       </c>
       <c r="G18">
-        <v>94.13188366941753</v>
+        <v>32.66685298763658</v>
       </c>
       <c r="H18">
-        <v>7.181405006869758</v>
+        <v>0.842300774244695</v>
       </c>
       <c r="I18">
-        <v>8.284209214304397</v>
+        <v>0.8318209175283011</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -871,16 +874,19 @@
         <v>17</v>
       </c>
       <c r="D19">
-        <v>1.174556091694368</v>
+        <v>10.01393036230197</v>
+      </c>
+      <c r="F19">
+        <v>86.98421602938777</v>
       </c>
       <c r="G19">
-        <v>96.87653309875202</v>
+        <v>41.40143943858133</v>
       </c>
       <c r="H19">
-        <v>9.267046536397418</v>
+        <v>0.9629324072346044</v>
       </c>
       <c r="I19">
-        <v>10.69012988861825</v>
+        <v>0.9509516588321826</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -891,16 +897,19 @@
         <v>18</v>
       </c>
       <c r="D20">
-        <v>1.343005795675444</v>
+        <v>12.73937992337878</v>
+      </c>
+      <c r="F20">
+        <v>87.14794195590076</v>
       </c>
       <c r="G20">
-        <v>98.44153763627349</v>
+        <v>50.71920943357676</v>
       </c>
       <c r="H20">
-        <v>11.87972964646743</v>
+        <v>1.100605953015493</v>
       </c>
       <c r="I20">
-        <v>13.70402667814547</v>
+        <v>1.08691227844995</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -911,16 +920,19 @@
         <v>19</v>
       </c>
       <c r="D21">
-        <v>1.535324388421378</v>
+        <v>16.04663307398143</v>
+      </c>
+      <c r="F21">
+        <v>87.22736879060132</v>
       </c>
       <c r="G21">
-        <v>99.31632953986316</v>
+        <v>59.99664561705126</v>
       </c>
       <c r="H21">
-        <v>15.1045272791822</v>
+        <v>1.257657291115191</v>
       </c>
       <c r="I21">
-        <v>17.42403665358163</v>
+        <v>1.242009593033667</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -931,16 +943,16 @@
         <v>20</v>
       </c>
       <c r="D22">
-        <v>1.754805416117448</v>
+        <v>19.97324198184441</v>
       </c>
       <c r="G22">
-        <v>99.79988186375152</v>
+        <v>68.62078218132146</v>
       </c>
       <c r="H22">
-        <v>19.01287999837558</v>
+        <v>1.43672066127139</v>
       </c>
       <c r="I22">
-        <v>21.93257106685047</v>
+        <v>1.418845067265071</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -951,16 +963,16 @@
         <v>21</v>
       </c>
       <c r="D23">
-        <v>2.005169850898939</v>
+        <v>24.51617550445877</v>
       </c>
       <c r="G23">
-        <v>100.0655224086089</v>
+        <v>76.14064018425847</v>
       </c>
       <c r="H23">
-        <v>23.64627443988324</v>
+        <v>1.640760121768081</v>
       </c>
       <c r="I23">
-        <v>27.27748740134577</v>
+        <v>1.620345880789232</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -971,16 +983,16 @@
         <v>22</v>
       </c>
       <c r="D24">
-        <v>2.290613300341976</v>
+        <v>29.61754540939863</v>
       </c>
       <c r="G24">
-        <v>100.2109566348107</v>
+        <v>82.3403466490788</v>
       </c>
       <c r="H24">
-        <v>28.99762995776731</v>
+        <v>1.87310224077475</v>
       </c>
       <c r="I24">
-        <v>33.45061767987289</v>
+        <v>1.849797212810033</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -991,16 +1003,16 @@
         <v>23</v>
       </c>
       <c r="D25">
-        <v>2.615855849310002</v>
+        <v>35.15743654223695</v>
       </c>
       <c r="G25">
-        <v>100.2904313056629</v>
+        <v>87.2198354713115</v>
       </c>
       <c r="H25">
-        <v>34.99493609046499</v>
+        <v>2.137469322800891</v>
       </c>
       <c r="I25">
-        <v>40.36889323708927</v>
+        <v>2.110875055143085</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1011,16 +1023,16 @@
         <v>24</v>
       </c>
       <c r="D26">
-        <v>2.986193782116025</v>
+        <v>40.95909960323701</v>
       </c>
       <c r="G26">
-        <v>100.3338171392718</v>
+        <v>90.92181660821086</v>
       </c>
       <c r="H26">
-        <v>41.49361220627869</v>
+        <v>2.438012170137351</v>
       </c>
       <c r="I26">
-        <v>47.86553108273419</v>
+        <v>2.407678566041148</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1031,13 +1043,16 @@
         <v>25</v>
       </c>
       <c r="D27">
-        <v>3.407552051962866</v>
+        <v>46.80847860549425</v>
+      </c>
+      <c r="G27">
+        <v>93.65296262455986</v>
       </c>
       <c r="H27">
-        <v>48.28360496128995</v>
+        <v>2.779341001449049</v>
       </c>
       <c r="I27">
-        <v>55.69822127251122</v>
+        <v>2.744760604099535</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1048,13 +1063,16 @@
         <v>26</v>
       </c>
       <c r="D28">
-        <v>3.886535879234977</v>
+        <v>52.48444630390529</v>
+      </c>
+      <c r="G28">
+        <v>95.62656580119416</v>
       </c>
       <c r="H28">
-        <v>55.11317624741073</v>
+        <v>3.16655268802832</v>
       </c>
       <c r="I28">
-        <v>63.5765678250463</v>
+        <v>3.127154625637595</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1065,13 +1083,16 @@
         <v>27</v>
       </c>
       <c r="D29">
-        <v>4.43047925457314</v>
+        <v>57.79117451115199</v>
+      </c>
+      <c r="G29">
+        <v>97.03149847953422</v>
       </c>
       <c r="H29">
-        <v>61.72471900046482</v>
+        <v>3.605251917884985</v>
       </c>
       <c r="I29">
-        <v>71.20340454337976</v>
+        <v>3.560395585466415</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1082,13 +1103,16 @@
         <v>28</v>
       </c>
       <c r="D30">
-        <v>5.047487383676582</v>
+        <v>62.58301845269438</v>
+      </c>
+      <c r="G30">
+        <v>98.02096335501528</v>
       </c>
       <c r="H30">
-        <v>67.89234630365254</v>
+        <v>4.101563260945936</v>
       </c>
       <c r="I30">
-        <v>78.31815644590949</v>
+        <v>4.050531851973906</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1099,13 +1123,16 @@
         <v>29</v>
       </c>
       <c r="D31">
-        <v>5.746469231579741</v>
+        <v>66.77588183103867</v>
+      </c>
+      <c r="G31">
+        <v>98.71257866991384</v>
       </c>
       <c r="H31">
-        <v>73.45012811469283</v>
+        <v>4.662130398349921</v>
       </c>
       <c r="I31">
-        <v>84.72941263408849</v>
+        <v>4.604124446008654</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1116,13 +1143,16 @@
         <v>30</v>
       </c>
       <c r="D32">
-        <v>6.537155309096799</v>
+        <v>70.3447960977855</v>
+      </c>
+      <c r="G32">
+        <v>99.19345468037042</v>
       </c>
       <c r="H32">
-        <v>78.30431276151138</v>
+        <v>5.294098024911536</v>
       </c>
       <c r="I32">
-        <v>90.32902456805424</v>
+        <v>5.228229168512386</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1133,13 +1163,16 @@
         <v>31</v>
       </c>
       <c r="D33">
-        <v>7.430094715627095</v>
+        <v>73.31195794778358</v>
+      </c>
+      <c r="G33">
+        <v>99.52657731652683</v>
       </c>
       <c r="H33">
-        <v>82.42962668190984</v>
+        <v>6.005071189266102</v>
       </c>
       <c r="I33">
-        <v>95.08783758007225</v>
+        <v>5.930356446552389</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1150,13 +1183,16 @@
         <v>32</v>
       </c>
       <c r="D34">
-        <v>8.436624259856019</v>
+        <v>75.73093940945242</v>
+      </c>
+      <c r="G34">
+        <v>99.7567574903606</v>
       </c>
       <c r="H34">
-        <v>85.85482697005199</v>
+        <v>6.803046184487737</v>
       </c>
       <c r="I34">
-        <v>99.03902481442562</v>
+        <v>6.718403083794434</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1167,13 +1203,16 @@
         <v>33</v>
       </c>
       <c r="D35">
-        <v>9.568801309831668</v>
+        <v>77.67169313536063</v>
+      </c>
+      <c r="G35">
+        <v>99.91552670169135</v>
       </c>
       <c r="H35">
-        <v>88.6441754707447</v>
+        <v>7.696306663989712</v>
       </c>
       <c r="I35">
-        <v>102.2567164122731</v>
+        <v>7.600549668922997</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1184,13 +1223,16 @@
         <v>34</v>
       </c>
       <c r="D36">
-        <v>10.83929101224055</v>
+        <v>79.20885916187824</v>
+      </c>
+      <c r="G36">
+        <v>100.0249063637965</v>
       </c>
       <c r="H36">
-        <v>90.88009816063207</v>
+        <v>8.693278596086341</v>
       </c>
       <c r="I36">
-        <v>104.8359960006431</v>
+        <v>8.585117334849969</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1201,13 +1243,16 @@
         <v>35</v>
       </c>
       <c r="D37">
-        <v>12.26119786298671</v>
+        <v>80.41400507621272</v>
+      </c>
+      <c r="G37">
+        <v>100.1001973506934</v>
       </c>
       <c r="H37">
-        <v>92.64980372601799</v>
+        <v>9.80233818964116</v>
       </c>
       <c r="I37">
-        <v>106.8774643675367</v>
+        <v>9.680378074140624</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1218,13 +1263,16 @@
         <v>36</v>
       </c>
       <c r="D38">
-        <v>13.84783156939231</v>
+        <v>81.35130882428949</v>
+      </c>
+      <c r="G38">
+        <v>100.1519936695917</v>
       </c>
       <c r="H38">
-        <v>94.03649115833471</v>
+        <v>11.03156825754877</v>
       </c>
       <c r="I38">
-        <v>108.4770968618981</v>
+        <v>10.89431413380669</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1235,13 +1283,13 @@
         <v>37</v>
       </c>
       <c r="D39">
-        <v>15.6123980447923</v>
+        <v>82.0757673825847</v>
       </c>
       <c r="H39">
-        <v>95.11452113220301</v>
+        <v>12.38846087569467</v>
       </c>
       <c r="I39">
-        <v>109.7206732698952</v>
+        <v>12.23432437376594</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1252,13 +1300,13 @@
         <v>38</v>
       </c>
       <c r="D40">
-        <v>17.56760859210218</v>
+        <v>82.6330205757063</v>
       </c>
       <c r="H40">
-        <v>95.94746911108324</v>
+        <v>13.87956784732541</v>
       </c>
       <c r="I40">
-        <v>110.6815319479777</v>
+        <v>13.70687908011412</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1269,13 +1317,13 @@
         <v>39</v>
       </c>
       <c r="D41">
-        <v>19.72520424357499</v>
+        <v>83.0600716807558</v>
       </c>
       <c r="H41">
-        <v>96.5880060623244</v>
+        <v>15.51010550105049</v>
       </c>
       <c r="I41">
-        <v>111.4204322200691</v>
+        <v>15.31712968020678</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1286,13 +1334,13 @@
         <v>40</v>
       </c>
       <c r="D42">
-        <v>22.09539814508831</v>
+        <v>83.38641253520511</v>
       </c>
       <c r="H42">
-        <v>97.07878388185348</v>
+        <v>17.2835266578664</v>
       </c>
       <c r="I42">
-        <v>111.9865757714814</v>
+        <v>17.06848603524459</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1303,13 +1351,13 @@
         <v>41</v>
       </c>
       <c r="D43">
-        <v>24.68624695378551</v>
+        <v>83.63525153485229</v>
       </c>
       <c r="H43">
-        <v>97.45376576547997</v>
+        <v>19.20107985182191</v>
       </c>
       <c r="I43">
-        <v>112.41914131716</v>
+        <v>18.96218114508907</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1320,13 +1368,13 @@
         <v>42</v>
       </c>
       <c r="D44">
-        <v>27.50297230956189</v>
+        <v>83.82467989301712</v>
       </c>
       <c r="H44">
-        <v>97.73966087177732</v>
+        <v>21.2613833915962</v>
       </c>
       <c r="I44">
-        <v>112.7489395769222</v>
+        <v>20.99685050934159</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1337,13 +1385,13 @@
         <v>43</v>
       </c>
       <c r="D45">
-        <v>30.54726496003173</v>
+        <v>83.9686999543857</v>
       </c>
       <c r="H45">
-        <v>97.95727883584112</v>
+        <v>23.46004855253364</v>
       </c>
       <c r="I45">
-        <v>112.9999757935637</v>
+        <v>23.16816000760067</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1354,13 +1402,13 @@
         <v>44</v>
       </c>
       <c r="D46">
-        <v>33.81661593581889</v>
+        <v>84.07809152750981</v>
       </c>
       <c r="H46">
-        <v>98.12271994308287</v>
+        <v>25.78939073484342</v>
       </c>
       <c r="I46">
-        <v>113.190822674324</v>
+        <v>25.46852065141437</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1371,13 +1419,13 @@
         <v>45</v>
       </c>
       <c r="D47">
-        <v>37.303729584225</v>
+        <v>84.16112015911541</v>
       </c>
       <c r="H47">
-        <v>98.24837559537637</v>
+        <v>28.23826833618244</v>
       </c>
       <c r="I47">
-        <v>113.3357744924659</v>
+        <v>27.88692946160092</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1388,13 +1436,13 @@
         <v>46</v>
       </c>
       <c r="D48">
-        <v>40.99608010787411</v>
+        <v>84.2241043233758</v>
       </c>
       <c r="H48">
-        <v>98.3437450124126</v>
+        <v>30.7920850675578</v>
       </c>
       <c r="I48">
-        <v>113.4457892044364</v>
+        <v>30.40897175533702</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1405,13 +1453,13 @@
         <v>47</v>
       </c>
       <c r="D49">
-        <v>44.87567419028723</v>
+        <v>84.2718630120345</v>
       </c>
       <c r="H49">
-        <v>98.41608855708702</v>
+        <v>33.43298175421227</v>
       </c>
       <c r="I49">
-        <v>113.5292421024158</v>
+        <v>33.01701056066785</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1422,13 +1470,13 @@
         <v>48</v>
       </c>
       <c r="D50">
-        <v>48.9190753162413</v>
+        <v>84.30806521924772</v>
       </c>
       <c r="H50">
-        <v>98.47094290706144</v>
+        <v>36.14022850570045</v>
       </c>
       <c r="I50">
-        <v>113.5925200976087</v>
+        <v>35.69057390722629</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1439,13 +1487,13 @@
         <v>49</v>
       </c>
       <c r="D51">
-        <v>53.09772943784277</v>
+        <v>84.33550071531724</v>
       </c>
       <c r="H51">
-        <v>98.51252308557143</v>
+        <v>38.89080887543376</v>
       </c>
       <c r="I51">
-        <v>113.6404854884501</v>
+        <v>38.40693171769913</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1455,14 +1503,11 @@
       <c r="B52">
         <v>50</v>
       </c>
-      <c r="D52">
-        <v>57.37860713570763</v>
-      </c>
       <c r="H52">
-        <v>98.54403381984859</v>
+        <v>41.66016675342269</v>
       </c>
       <c r="I52">
-        <v>113.6768351324262</v>
+        <v>41.14183340777375</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1472,14 +1517,11 @@
       <c r="B53">
         <v>51</v>
       </c>
-      <c r="D53">
-        <v>61.72514666984176</v>
-      </c>
       <c r="H53">
-        <v>98.56790932454847</v>
+        <v>44.42306749980694</v>
       </c>
       <c r="I53">
-        <v>113.704377051569</v>
+        <v>43.87035830549552</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -1489,8 +1531,11 @@
       <c r="B54">
         <v>52</v>
       </c>
-      <c r="D54">
-        <v>66.09844935809443</v>
+      <c r="H54">
+        <v>47.15451057925244</v>
+      </c>
+      <c r="I54">
+        <v>46.56781693072127</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -1500,8 +1545,11 @@
       <c r="B55">
         <v>53</v>
       </c>
-      <c r="D55">
-        <v>70.45864874858137</v>
+      <c r="H55">
+        <v>49.83062434787065</v>
+      </c>
+      <c r="I55">
+        <v>49.21063464915238</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -1511,8 +1559,11 @@
       <c r="B56">
         <v>54</v>
       </c>
-      <c r="D56">
-        <v>74.76635331514841</v>
+      <c r="H56">
+        <v>52.42947594708044</v>
+      </c>
+      <c r="I56">
+        <v>51.7771514895448</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -1522,8 +1573,11 @@
       <c r="B57">
         <v>55</v>
       </c>
-      <c r="D57">
-        <v>78.98405295972628</v>
+      <c r="H57">
+        <v>54.93174002660821</v>
+      </c>
+      <c r="I57">
+        <v>54.24828254649695</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -1533,8 +1587,11 @@
       <c r="B58">
         <v>56</v>
       </c>
-      <c r="D58">
-        <v>83.07738427300244</v>
+      <c r="H58">
+        <v>57.32118720728107</v>
+      </c>
+      <c r="I58">
+        <v>56.6080003658175</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -1544,8 +1601,11 @@
       <c r="B59">
         <v>57</v>
       </c>
-      <c r="D59">
-        <v>87.01616738134429</v>
+      <c r="H59">
+        <v>59.58497369853135</v>
+      </c>
+      <c r="I59">
+        <v>58.843620958626</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -1555,8 +1615,11 @@
       <c r="B60">
         <v>58</v>
       </c>
-      <c r="D60">
-        <v>90.77515490811717</v>
+      <c r="H60">
+        <v>61.71373390992727</v>
+      </c>
+      <c r="I60">
+        <v>60.94589526061623</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -1566,8 +1629,11 @@
       <c r="B61">
         <v>59</v>
       </c>
-      <c r="D61">
-        <v>94.33446612242822</v>
+      <c r="H61">
+        <v>63.70149530819895</v>
+      </c>
+      <c r="I61">
+        <v>62.90892504842614</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -1577,8 +1643,11 @@
       <c r="B62">
         <v>60</v>
       </c>
-      <c r="D62">
-        <v>97.67971139206344</v>
+      <c r="H62">
+        <v>65.54544722960019</v>
+      </c>
+      <c r="I62">
+        <v>64.72993462842263</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -1588,8 +1657,11 @@
       <c r="B63">
         <v>61</v>
       </c>
-      <c r="D63">
-        <v>100.8018390616198</v>
+      <c r="H63">
+        <v>67.24560210863305</v>
+      </c>
+      <c r="I63">
+        <v>66.40893628039842</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -1599,118 +1671,151 @@
       <c r="B64">
         <v>62</v>
       </c>
-      <c r="D64">
-        <v>103.6967559087457</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="H64">
+        <v>68.80438894835403</v>
+      </c>
+      <c r="I64">
+        <v>67.94832878589678</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65">
         <v>63</v>
       </c>
-      <c r="D65">
-        <v>106.3647823362227</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="H65">
+        <v>70.22621590769158</v>
+      </c>
+      <c r="I65">
+        <v>69.35246545779192</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66">
         <v>64</v>
       </c>
-      <c r="D66">
-        <v>108.8100050472854</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="H66">
+        <v>71.51703305141109</v>
+      </c>
+      <c r="I66">
+        <v>70.62722233049318</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67">
         <v>65</v>
       </c>
-      <c r="D67">
-        <v>111.0395848828597</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="H67">
+        <v>72.68391904425475</v>
+      </c>
+      <c r="I67">
+        <v>71.7795899964122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68">
         <v>66</v>
       </c>
-      <c r="D68">
-        <v>113.0630680548102</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="H68">
+        <v>73.73470808856941</v>
+      </c>
+      <c r="I68">
+        <v>72.81730518521074</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69">
         <v>67</v>
       </c>
-      <c r="D69">
-        <v>114.8917374555697</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="H69">
+        <v>74.67766657332118</v>
+      </c>
+      <c r="I69">
+        <v>73.74853143592941</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70">
         <v>68</v>
       </c>
-      <c r="D70">
-        <v>116.5380289460816</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="H70">
+        <v>75.5212232290225</v>
+      </c>
+      <c r="I70">
+        <v>74.58159260931109</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71">
         <v>69</v>
       </c>
-      <c r="D71">
-        <v>118.0150268502754</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="H71">
+        <v>76.27375226619912</v>
+      </c>
+      <c r="I71">
+        <v>75.32475872444645</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72">
         <v>70</v>
       </c>
-      <c r="D72">
-        <v>119.3360440769569</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="H72">
+        <v>76.94340598795233</v>
+      </c>
+      <c r="I72">
+        <v>75.98608065396088</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73">
         <v>71</v>
       </c>
-      <c r="D73">
-        <v>120.5142856317051</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="H73">
+        <v>77.53799154493252</v>
+      </c>
+      <c r="I73">
+        <v>76.57326841239534</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74">
         <v>72</v>
       </c>
-      <c r="D74">
-        <v>121.5625897096425</v>
+      <c r="H74">
+        <v>78.06488561353471</v>
+      </c>
+      <c r="I74">
+        <v>77.09360689597075</v>
       </c>
     </row>
   </sheetData>

</xml_diff>